<commit_message>
Reason append with RPA and submit exception handling
</commit_message>
<xml_diff>
--- a/Inputs/New Microsoft Excel Worksheet.xlsx
+++ b/Inputs/New Microsoft Excel Worksheet.xlsx
@@ -193,15 +193,6 @@
     <x:t>n/a</x:t>
   </x:si>
   <x:si>
-    <x:t>Delivery Feast</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32980</x:t>
-  </x:si>
-  <x:si>
-    <x:t>33211</x:t>
-  </x:si>
-  <x:si>
     <x:t>Burger Feast</x:t>
   </x:si>
   <x:si>
@@ -265,12 +256,6 @@
     <x:t>33215</x:t>
   </x:si>
   <x:si>
-    <x:t>My Bucket</x:t>
-  </x:si>
-  <x:si>
-    <x:t>33238</x:t>
-  </x:si>
-  <x:si>
     <x:t>33006</x:t>
   </x:si>
   <x:si>
@@ -536,18 +521,6 @@
   </x:si>
   <x:si>
     <x:t>32901</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Regular Chips</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32902</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Large Chips</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32903</x:t>
   </x:si>
   <x:si>
     <x:t>Regular Potato &amp; Gravy</x:t>
@@ -1593,29 +1566,29 @@
         <x:v>66</x:v>
       </x:c>
       <x:c r="C25" s="0" t="s">
-        <x:v>67</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:3">
       <x:c r="A26" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="B26" s="0" t="s">
         <x:v>68</x:v>
       </x:c>
-      <x:c r="B26" s="0" t="s">
-        <x:v>69</x:v>
-      </x:c>
       <x:c r="C26" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:3">
       <x:c r="A27" s="0" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="B27" s="0" t="s">
         <x:v>70</x:v>
       </x:c>
-      <x:c r="B27" s="0" t="s">
+      <x:c r="C27" s="0" t="s">
         <x:v>71</x:v>
-      </x:c>
-      <x:c r="C27" s="0" t="s">
-        <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:3">
@@ -1626,37 +1599,37 @@
         <x:v>73</x:v>
       </x:c>
       <x:c r="C28" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:3">
       <x:c r="A29" s="0" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="B29" s="0" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="B29" s="0" t="s">
-        <x:v>76</x:v>
-      </x:c>
       <x:c r="C29" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:3">
       <x:c r="A30" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="B30" s="0" t="s">
         <x:v>77</x:v>
       </x:c>
-      <x:c r="B30" s="0" t="s">
-        <x:v>78</x:v>
-      </x:c>
       <x:c r="C30" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:3">
       <x:c r="A31" s="0" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="B31" s="0" t="s">
         <x:v>79</x:v>
-      </x:c>
-      <x:c r="B31" s="0" t="s">
-        <x:v>80</x:v>
       </x:c>
       <x:c r="C31" s="0" t="s">
         <x:v>5</x:v>
@@ -1664,76 +1637,76 @@
     </x:row>
     <x:row r="32" spans="1:3">
       <x:c r="A32" s="0" t="s">
-        <x:v>81</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
-        <x:v>82</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="C32" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>80</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:3">
       <x:c r="A33" s="0" t="s">
-        <x:v>83</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
-        <x:v>84</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="C33" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>82</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:3">
       <x:c r="A34" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
         <x:v>58</x:v>
       </x:c>
       <x:c r="C34" s="0" t="s">
-        <x:v>85</x:v>
+        <x:v>84</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:3">
       <x:c r="A35" s="0" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="B35" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="C35" s="0" t="s">
         <x:v>86</x:v>
-      </x:c>
-      <x:c r="B35" s="0" t="s">
-        <x:v>58</x:v>
-      </x:c>
-      <x:c r="C35" s="0" t="s">
-        <x:v>87</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:3">
       <x:c r="A36" s="0" t="s">
+        <x:v>87</x:v>
+      </x:c>
+      <x:c r="B36" s="0" t="s">
         <x:v>88</x:v>
       </x:c>
-      <x:c r="B36" s="0" t="s">
-        <x:v>58</x:v>
-      </x:c>
       <x:c r="C36" s="0" t="s">
-        <x:v>89</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:3">
       <x:c r="A37" s="0" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="B37" s="0" t="s">
         <x:v>90</x:v>
       </x:c>
-      <x:c r="B37" s="0" t="s">
-        <x:v>58</x:v>
-      </x:c>
       <x:c r="C37" s="0" t="s">
-        <x:v>91</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:3">
       <x:c r="A38" s="0" t="s">
+        <x:v>91</x:v>
+      </x:c>
+      <x:c r="B38" s="0" t="s">
         <x:v>92</x:v>
-      </x:c>
-      <x:c r="B38" s="0" t="s">
-        <x:v>93</x:v>
       </x:c>
       <x:c r="C38" s="0" t="s">
         <x:v>5</x:v>
@@ -1741,10 +1714,10 @@
     </x:row>
     <x:row r="39" spans="1:3">
       <x:c r="A39" s="0" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="B39" s="0" t="s">
         <x:v>94</x:v>
-      </x:c>
-      <x:c r="B39" s="0" t="s">
-        <x:v>95</x:v>
       </x:c>
       <x:c r="C39" s="0" t="s">
         <x:v>5</x:v>
@@ -1752,10 +1725,10 @@
     </x:row>
     <x:row r="40" spans="1:3">
       <x:c r="A40" s="0" t="s">
+        <x:v>95</x:v>
+      </x:c>
+      <x:c r="B40" s="0" t="s">
         <x:v>96</x:v>
-      </x:c>
-      <x:c r="B40" s="0" t="s">
-        <x:v>97</x:v>
       </x:c>
       <x:c r="C40" s="0" t="s">
         <x:v>5</x:v>
@@ -1763,10 +1736,10 @@
     </x:row>
     <x:row r="41" spans="1:3">
       <x:c r="A41" s="0" t="s">
+        <x:v>97</x:v>
+      </x:c>
+      <x:c r="B41" s="0" t="s">
         <x:v>98</x:v>
-      </x:c>
-      <x:c r="B41" s="0" t="s">
-        <x:v>99</x:v>
       </x:c>
       <x:c r="C41" s="0" t="s">
         <x:v>5</x:v>
@@ -1774,10 +1747,10 @@
     </x:row>
     <x:row r="42" spans="1:3">
       <x:c r="A42" s="0" t="s">
+        <x:v>99</x:v>
+      </x:c>
+      <x:c r="B42" s="0" t="s">
         <x:v>100</x:v>
-      </x:c>
-      <x:c r="B42" s="0" t="s">
-        <x:v>101</x:v>
       </x:c>
       <x:c r="C42" s="0" t="s">
         <x:v>5</x:v>
@@ -1785,10 +1758,10 @@
     </x:row>
     <x:row r="43" spans="1:3">
       <x:c r="A43" s="0" t="s">
+        <x:v>101</x:v>
+      </x:c>
+      <x:c r="B43" s="0" t="s">
         <x:v>102</x:v>
-      </x:c>
-      <x:c r="B43" s="0" t="s">
-        <x:v>103</x:v>
       </x:c>
       <x:c r="C43" s="0" t="s">
         <x:v>5</x:v>
@@ -1796,10 +1769,10 @@
     </x:row>
     <x:row r="44" spans="1:3">
       <x:c r="A44" s="0" t="s">
+        <x:v>103</x:v>
+      </x:c>
+      <x:c r="B44" s="0" t="s">
         <x:v>104</x:v>
-      </x:c>
-      <x:c r="B44" s="0" t="s">
-        <x:v>105</x:v>
       </x:c>
       <x:c r="C44" s="0" t="s">
         <x:v>5</x:v>
@@ -1807,10 +1780,10 @@
     </x:row>
     <x:row r="45" spans="1:3">
       <x:c r="A45" s="0" t="s">
+        <x:v>105</x:v>
+      </x:c>
+      <x:c r="B45" s="0" t="s">
         <x:v>106</x:v>
-      </x:c>
-      <x:c r="B45" s="0" t="s">
-        <x:v>107</x:v>
       </x:c>
       <x:c r="C45" s="0" t="s">
         <x:v>5</x:v>
@@ -1818,10 +1791,10 @@
     </x:row>
     <x:row r="46" spans="1:3">
       <x:c r="A46" s="0" t="s">
+        <x:v>107</x:v>
+      </x:c>
+      <x:c r="B46" s="0" t="s">
         <x:v>108</x:v>
-      </x:c>
-      <x:c r="B46" s="0" t="s">
-        <x:v>109</x:v>
       </x:c>
       <x:c r="C46" s="0" t="s">
         <x:v>5</x:v>
@@ -1829,10 +1802,10 @@
     </x:row>
     <x:row r="47" spans="1:3">
       <x:c r="A47" s="0" t="s">
+        <x:v>109</x:v>
+      </x:c>
+      <x:c r="B47" s="0" t="s">
         <x:v>110</x:v>
-      </x:c>
-      <x:c r="B47" s="0" t="s">
-        <x:v>111</x:v>
       </x:c>
       <x:c r="C47" s="0" t="s">
         <x:v>5</x:v>
@@ -1840,10 +1813,10 @@
     </x:row>
     <x:row r="48" spans="1:3">
       <x:c r="A48" s="0" t="s">
+        <x:v>111</x:v>
+      </x:c>
+      <x:c r="B48" s="0" t="s">
         <x:v>112</x:v>
-      </x:c>
-      <x:c r="B48" s="0" t="s">
-        <x:v>113</x:v>
       </x:c>
       <x:c r="C48" s="0" t="s">
         <x:v>5</x:v>
@@ -1851,10 +1824,10 @@
     </x:row>
     <x:row r="49" spans="1:3">
       <x:c r="A49" s="0" t="s">
+        <x:v>113</x:v>
+      </x:c>
+      <x:c r="B49" s="0" t="s">
         <x:v>114</x:v>
-      </x:c>
-      <x:c r="B49" s="0" t="s">
-        <x:v>115</x:v>
       </x:c>
       <x:c r="C49" s="0" t="s">
         <x:v>5</x:v>
@@ -1862,10 +1835,10 @@
     </x:row>
     <x:row r="50" spans="1:3">
       <x:c r="A50" s="0" t="s">
+        <x:v>115</x:v>
+      </x:c>
+      <x:c r="B50" s="0" t="s">
         <x:v>116</x:v>
-      </x:c>
-      <x:c r="B50" s="0" t="s">
-        <x:v>117</x:v>
       </x:c>
       <x:c r="C50" s="0" t="s">
         <x:v>5</x:v>
@@ -1873,10 +1846,10 @@
     </x:row>
     <x:row r="51" spans="1:3">
       <x:c r="A51" s="0" t="s">
+        <x:v>117</x:v>
+      </x:c>
+      <x:c r="B51" s="0" t="s">
         <x:v>118</x:v>
-      </x:c>
-      <x:c r="B51" s="0" t="s">
-        <x:v>119</x:v>
       </x:c>
       <x:c r="C51" s="0" t="s">
         <x:v>5</x:v>
@@ -1884,10 +1857,10 @@
     </x:row>
     <x:row r="52" spans="1:3">
       <x:c r="A52" s="0" t="s">
+        <x:v>119</x:v>
+      </x:c>
+      <x:c r="B52" s="0" t="s">
         <x:v>120</x:v>
-      </x:c>
-      <x:c r="B52" s="0" t="s">
-        <x:v>121</x:v>
       </x:c>
       <x:c r="C52" s="0" t="s">
         <x:v>5</x:v>
@@ -1895,10 +1868,10 @@
     </x:row>
     <x:row r="53" spans="1:3">
       <x:c r="A53" s="0" t="s">
+        <x:v>121</x:v>
+      </x:c>
+      <x:c r="B53" s="0" t="s">
         <x:v>122</x:v>
-      </x:c>
-      <x:c r="B53" s="0" t="s">
-        <x:v>123</x:v>
       </x:c>
       <x:c r="C53" s="0" t="s">
         <x:v>5</x:v>
@@ -1906,10 +1879,10 @@
     </x:row>
     <x:row r="54" spans="1:3">
       <x:c r="A54" s="0" t="s">
+        <x:v>123</x:v>
+      </x:c>
+      <x:c r="B54" s="0" t="s">
         <x:v>124</x:v>
-      </x:c>
-      <x:c r="B54" s="0" t="s">
-        <x:v>125</x:v>
       </x:c>
       <x:c r="C54" s="0" t="s">
         <x:v>5</x:v>
@@ -1917,10 +1890,10 @@
     </x:row>
     <x:row r="55" spans="1:3">
       <x:c r="A55" s="0" t="s">
+        <x:v>125</x:v>
+      </x:c>
+      <x:c r="B55" s="0" t="s">
         <x:v>126</x:v>
-      </x:c>
-      <x:c r="B55" s="0" t="s">
-        <x:v>127</x:v>
       </x:c>
       <x:c r="C55" s="0" t="s">
         <x:v>5</x:v>
@@ -1928,10 +1901,10 @@
     </x:row>
     <x:row r="56" spans="1:3">
       <x:c r="A56" s="0" t="s">
+        <x:v>127</x:v>
+      </x:c>
+      <x:c r="B56" s="0" t="s">
         <x:v>128</x:v>
-      </x:c>
-      <x:c r="B56" s="0" t="s">
-        <x:v>129</x:v>
       </x:c>
       <x:c r="C56" s="0" t="s">
         <x:v>5</x:v>
@@ -1939,10 +1912,10 @@
     </x:row>
     <x:row r="57" spans="1:3">
       <x:c r="A57" s="0" t="s">
+        <x:v>129</x:v>
+      </x:c>
+      <x:c r="B57" s="0" t="s">
         <x:v>130</x:v>
-      </x:c>
-      <x:c r="B57" s="0" t="s">
-        <x:v>131</x:v>
       </x:c>
       <x:c r="C57" s="0" t="s">
         <x:v>5</x:v>
@@ -1950,10 +1923,10 @@
     </x:row>
     <x:row r="58" spans="1:3">
       <x:c r="A58" s="0" t="s">
+        <x:v>131</x:v>
+      </x:c>
+      <x:c r="B58" s="0" t="s">
         <x:v>132</x:v>
-      </x:c>
-      <x:c r="B58" s="0" t="s">
-        <x:v>133</x:v>
       </x:c>
       <x:c r="C58" s="0" t="s">
         <x:v>5</x:v>
@@ -1961,10 +1934,10 @@
     </x:row>
     <x:row r="59" spans="1:3">
       <x:c r="A59" s="0" t="s">
+        <x:v>133</x:v>
+      </x:c>
+      <x:c r="B59" s="0" t="s">
         <x:v>134</x:v>
-      </x:c>
-      <x:c r="B59" s="0" t="s">
-        <x:v>135</x:v>
       </x:c>
       <x:c r="C59" s="0" t="s">
         <x:v>5</x:v>
@@ -1972,10 +1945,10 @@
     </x:row>
     <x:row r="60" spans="1:3">
       <x:c r="A60" s="0" t="s">
+        <x:v>135</x:v>
+      </x:c>
+      <x:c r="B60" s="0" t="s">
         <x:v>136</x:v>
-      </x:c>
-      <x:c r="B60" s="0" t="s">
-        <x:v>137</x:v>
       </x:c>
       <x:c r="C60" s="0" t="s">
         <x:v>5</x:v>
@@ -1983,10 +1956,10 @@
     </x:row>
     <x:row r="61" spans="1:3">
       <x:c r="A61" s="0" t="s">
+        <x:v>137</x:v>
+      </x:c>
+      <x:c r="B61" s="0" t="s">
         <x:v>138</x:v>
-      </x:c>
-      <x:c r="B61" s="0" t="s">
-        <x:v>139</x:v>
       </x:c>
       <x:c r="C61" s="0" t="s">
         <x:v>5</x:v>
@@ -1994,10 +1967,10 @@
     </x:row>
     <x:row r="62" spans="1:3">
       <x:c r="A62" s="0" t="s">
+        <x:v>139</x:v>
+      </x:c>
+      <x:c r="B62" s="0" t="s">
         <x:v>140</x:v>
-      </x:c>
-      <x:c r="B62" s="0" t="s">
-        <x:v>141</x:v>
       </x:c>
       <x:c r="C62" s="0" t="s">
         <x:v>5</x:v>
@@ -2005,10 +1978,10 @@
     </x:row>
     <x:row r="63" spans="1:3">
       <x:c r="A63" s="0" t="s">
+        <x:v>141</x:v>
+      </x:c>
+      <x:c r="B63" s="0" t="s">
         <x:v>142</x:v>
-      </x:c>
-      <x:c r="B63" s="0" t="s">
-        <x:v>143</x:v>
       </x:c>
       <x:c r="C63" s="0" t="s">
         <x:v>5</x:v>
@@ -2016,10 +1989,10 @@
     </x:row>
     <x:row r="64" spans="1:3">
       <x:c r="A64" s="0" t="s">
+        <x:v>143</x:v>
+      </x:c>
+      <x:c r="B64" s="0" t="s">
         <x:v>144</x:v>
-      </x:c>
-      <x:c r="B64" s="0" t="s">
-        <x:v>145</x:v>
       </x:c>
       <x:c r="C64" s="0" t="s">
         <x:v>5</x:v>
@@ -2027,10 +2000,10 @@
     </x:row>
     <x:row r="65" spans="1:3">
       <x:c r="A65" s="0" t="s">
+        <x:v>145</x:v>
+      </x:c>
+      <x:c r="B65" s="0" t="s">
         <x:v>146</x:v>
-      </x:c>
-      <x:c r="B65" s="0" t="s">
-        <x:v>147</x:v>
       </x:c>
       <x:c r="C65" s="0" t="s">
         <x:v>5</x:v>
@@ -2038,10 +2011,10 @@
     </x:row>
     <x:row r="66" spans="1:3">
       <x:c r="A66" s="0" t="s">
+        <x:v>147</x:v>
+      </x:c>
+      <x:c r="B66" s="0" t="s">
         <x:v>148</x:v>
-      </x:c>
-      <x:c r="B66" s="0" t="s">
-        <x:v>149</x:v>
       </x:c>
       <x:c r="C66" s="0" t="s">
         <x:v>5</x:v>
@@ -2049,10 +2022,10 @@
     </x:row>
     <x:row r="67" spans="1:3">
       <x:c r="A67" s="0" t="s">
+        <x:v>149</x:v>
+      </x:c>
+      <x:c r="B67" s="0" t="s">
         <x:v>150</x:v>
-      </x:c>
-      <x:c r="B67" s="0" t="s">
-        <x:v>151</x:v>
       </x:c>
       <x:c r="C67" s="0" t="s">
         <x:v>5</x:v>
@@ -2060,10 +2033,10 @@
     </x:row>
     <x:row r="68" spans="1:3">
       <x:c r="A68" s="0" t="s">
+        <x:v>151</x:v>
+      </x:c>
+      <x:c r="B68" s="0" t="s">
         <x:v>152</x:v>
-      </x:c>
-      <x:c r="B68" s="0" t="s">
-        <x:v>153</x:v>
       </x:c>
       <x:c r="C68" s="0" t="s">
         <x:v>5</x:v>
@@ -2071,10 +2044,10 @@
     </x:row>
     <x:row r="69" spans="1:3">
       <x:c r="A69" s="0" t="s">
+        <x:v>153</x:v>
+      </x:c>
+      <x:c r="B69" s="0" t="s">
         <x:v>154</x:v>
-      </x:c>
-      <x:c r="B69" s="0" t="s">
-        <x:v>155</x:v>
       </x:c>
       <x:c r="C69" s="0" t="s">
         <x:v>5</x:v>
@@ -2082,10 +2055,10 @@
     </x:row>
     <x:row r="70" spans="1:3">
       <x:c r="A70" s="0" t="s">
+        <x:v>155</x:v>
+      </x:c>
+      <x:c r="B70" s="0" t="s">
         <x:v>156</x:v>
-      </x:c>
-      <x:c r="B70" s="0" t="s">
-        <x:v>157</x:v>
       </x:c>
       <x:c r="C70" s="0" t="s">
         <x:v>5</x:v>
@@ -2093,10 +2066,10 @@
     </x:row>
     <x:row r="71" spans="1:3">
       <x:c r="A71" s="0" t="s">
+        <x:v>157</x:v>
+      </x:c>
+      <x:c r="B71" s="0" t="s">
         <x:v>158</x:v>
-      </x:c>
-      <x:c r="B71" s="0" t="s">
-        <x:v>159</x:v>
       </x:c>
       <x:c r="C71" s="0" t="s">
         <x:v>5</x:v>
@@ -2104,10 +2077,10 @@
     </x:row>
     <x:row r="72" spans="1:3">
       <x:c r="A72" s="0" t="s">
+        <x:v>159</x:v>
+      </x:c>
+      <x:c r="B72" s="0" t="s">
         <x:v>160</x:v>
-      </x:c>
-      <x:c r="B72" s="0" t="s">
-        <x:v>161</x:v>
       </x:c>
       <x:c r="C72" s="0" t="s">
         <x:v>5</x:v>
@@ -2115,10 +2088,10 @@
     </x:row>
     <x:row r="73" spans="1:3">
       <x:c r="A73" s="0" t="s">
+        <x:v>161</x:v>
+      </x:c>
+      <x:c r="B73" s="0" t="s">
         <x:v>162</x:v>
-      </x:c>
-      <x:c r="B73" s="0" t="s">
-        <x:v>163</x:v>
       </x:c>
       <x:c r="C73" s="0" t="s">
         <x:v>5</x:v>
@@ -2126,10 +2099,10 @@
     </x:row>
     <x:row r="74" spans="1:3">
       <x:c r="A74" s="0" t="s">
+        <x:v>163</x:v>
+      </x:c>
+      <x:c r="B74" s="0" t="s">
         <x:v>164</x:v>
-      </x:c>
-      <x:c r="B74" s="0" t="s">
-        <x:v>165</x:v>
       </x:c>
       <x:c r="C74" s="0" t="s">
         <x:v>5</x:v>
@@ -2137,10 +2110,10 @@
     </x:row>
     <x:row r="75" spans="1:3">
       <x:c r="A75" s="0" t="s">
+        <x:v>165</x:v>
+      </x:c>
+      <x:c r="B75" s="0" t="s">
         <x:v>166</x:v>
-      </x:c>
-      <x:c r="B75" s="0" t="s">
-        <x:v>167</x:v>
       </x:c>
       <x:c r="C75" s="0" t="s">
         <x:v>5</x:v>
@@ -2148,10 +2121,10 @@
     </x:row>
     <x:row r="76" spans="1:3">
       <x:c r="A76" s="0" t="s">
+        <x:v>167</x:v>
+      </x:c>
+      <x:c r="B76" s="0" t="s">
         <x:v>168</x:v>
-      </x:c>
-      <x:c r="B76" s="0" t="s">
-        <x:v>169</x:v>
       </x:c>
       <x:c r="C76" s="0" t="s">
         <x:v>5</x:v>
@@ -2159,32 +2132,32 @@
     </x:row>
     <x:row r="77" spans="1:3">
       <x:c r="A77" s="0" t="s">
+        <x:v>169</x:v>
+      </x:c>
+      <x:c r="B77" s="0" t="s">
         <x:v>170</x:v>
       </x:c>
-      <x:c r="B77" s="0" t="s">
-        <x:v>171</x:v>
-      </x:c>
       <x:c r="C77" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="78" spans="1:3">
       <x:c r="A78" s="0" t="s">
+        <x:v>171</x:v>
+      </x:c>
+      <x:c r="B78" s="0" t="s">
         <x:v>172</x:v>
       </x:c>
-      <x:c r="B78" s="0" t="s">
-        <x:v>173</x:v>
-      </x:c>
       <x:c r="C78" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="79" spans="1:3">
       <x:c r="A79" s="0" t="s">
+        <x:v>173</x:v>
+      </x:c>
+      <x:c r="B79" s="0" t="s">
         <x:v>174</x:v>
-      </x:c>
-      <x:c r="B79" s="0" t="s">
-        <x:v>175</x:v>
       </x:c>
       <x:c r="C79" s="0" t="s">
         <x:v>5</x:v>
@@ -2192,43 +2165,43 @@
     </x:row>
     <x:row r="80" spans="1:3">
       <x:c r="A80" s="0" t="s">
+        <x:v>175</x:v>
+      </x:c>
+      <x:c r="B80" s="0" t="s">
         <x:v>176</x:v>
       </x:c>
-      <x:c r="B80" s="0" t="s">
-        <x:v>177</x:v>
-      </x:c>
       <x:c r="C80" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="81" spans="1:3">
       <x:c r="A81" s="0" t="s">
+        <x:v>177</x:v>
+      </x:c>
+      <x:c r="B81" s="0" t="s">
         <x:v>178</x:v>
       </x:c>
-      <x:c r="B81" s="0" t="s">
-        <x:v>179</x:v>
-      </x:c>
       <x:c r="C81" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="82" spans="1:3">
       <x:c r="A82" s="0" t="s">
+        <x:v>179</x:v>
+      </x:c>
+      <x:c r="B82" s="0" t="s">
         <x:v>180</x:v>
       </x:c>
-      <x:c r="B82" s="0" t="s">
-        <x:v>181</x:v>
-      </x:c>
       <x:c r="C82" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="83" spans="1:3">
       <x:c r="A83" s="0" t="s">
+        <x:v>181</x:v>
+      </x:c>
+      <x:c r="B83" s="0" t="s">
         <x:v>182</x:v>
-      </x:c>
-      <x:c r="B83" s="0" t="s">
-        <x:v>183</x:v>
       </x:c>
       <x:c r="C83" s="0" t="s">
         <x:v>5</x:v>
@@ -2236,21 +2209,21 @@
     </x:row>
     <x:row r="84" spans="1:3">
       <x:c r="A84" s="0" t="s">
+        <x:v>183</x:v>
+      </x:c>
+      <x:c r="B84" s="0" t="s">
         <x:v>184</x:v>
       </x:c>
-      <x:c r="B84" s="0" t="s">
-        <x:v>185</x:v>
-      </x:c>
       <x:c r="C84" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="85" spans="1:3">
       <x:c r="A85" s="0" t="s">
+        <x:v>185</x:v>
+      </x:c>
+      <x:c r="B85" s="0" t="s">
         <x:v>186</x:v>
-      </x:c>
-      <x:c r="B85" s="0" t="s">
-        <x:v>187</x:v>
       </x:c>
       <x:c r="C85" s="0" t="s">
         <x:v>5</x:v>
@@ -2258,10 +2231,10 @@
     </x:row>
     <x:row r="86" spans="1:3">
       <x:c r="A86" s="0" t="s">
+        <x:v>187</x:v>
+      </x:c>
+      <x:c r="B86" s="0" t="s">
         <x:v>188</x:v>
-      </x:c>
-      <x:c r="B86" s="0" t="s">
-        <x:v>189</x:v>
       </x:c>
       <x:c r="C86" s="0" t="s">
         <x:v>5</x:v>
@@ -2269,10 +2242,10 @@
     </x:row>
     <x:row r="87" spans="1:3">
       <x:c r="A87" s="0" t="s">
+        <x:v>189</x:v>
+      </x:c>
+      <x:c r="B87" s="0" t="s">
         <x:v>190</x:v>
-      </x:c>
-      <x:c r="B87" s="0" t="s">
-        <x:v>191</x:v>
       </x:c>
       <x:c r="C87" s="0" t="s">
         <x:v>5</x:v>
@@ -2280,10 +2253,10 @@
     </x:row>
     <x:row r="88" spans="1:3">
       <x:c r="A88" s="0" t="s">
+        <x:v>191</x:v>
+      </x:c>
+      <x:c r="B88" s="0" t="s">
         <x:v>192</x:v>
-      </x:c>
-      <x:c r="B88" s="0" t="s">
-        <x:v>193</x:v>
       </x:c>
       <x:c r="C88" s="0" t="s">
         <x:v>5</x:v>
@@ -2291,10 +2264,10 @@
     </x:row>
     <x:row r="89" spans="1:3">
       <x:c r="A89" s="0" t="s">
+        <x:v>193</x:v>
+      </x:c>
+      <x:c r="B89" s="0" t="s">
         <x:v>194</x:v>
-      </x:c>
-      <x:c r="B89" s="0" t="s">
-        <x:v>195</x:v>
       </x:c>
       <x:c r="C89" s="0" t="s">
         <x:v>5</x:v>
@@ -2302,10 +2275,10 @@
     </x:row>
     <x:row r="90" spans="1:3">
       <x:c r="A90" s="0" t="s">
+        <x:v>195</x:v>
+      </x:c>
+      <x:c r="B90" s="0" t="s">
         <x:v>196</x:v>
-      </x:c>
-      <x:c r="B90" s="0" t="s">
-        <x:v>197</x:v>
       </x:c>
       <x:c r="C90" s="0" t="s">
         <x:v>5</x:v>
@@ -2313,10 +2286,10 @@
     </x:row>
     <x:row r="91" spans="1:3">
       <x:c r="A91" s="0" t="s">
+        <x:v>197</x:v>
+      </x:c>
+      <x:c r="B91" s="0" t="s">
         <x:v>198</x:v>
-      </x:c>
-      <x:c r="B91" s="0" t="s">
-        <x:v>199</x:v>
       </x:c>
       <x:c r="C91" s="0" t="s">
         <x:v>5</x:v>
@@ -2324,10 +2297,10 @@
     </x:row>
     <x:row r="92" spans="1:3">
       <x:c r="A92" s="0" t="s">
+        <x:v>199</x:v>
+      </x:c>
+      <x:c r="B92" s="0" t="s">
         <x:v>200</x:v>
-      </x:c>
-      <x:c r="B92" s="0" t="s">
-        <x:v>201</x:v>
       </x:c>
       <x:c r="C92" s="0" t="s">
         <x:v>5</x:v>
@@ -2335,10 +2308,10 @@
     </x:row>
     <x:row r="93" spans="1:3">
       <x:c r="A93" s="0" t="s">
+        <x:v>201</x:v>
+      </x:c>
+      <x:c r="B93" s="0" t="s">
         <x:v>202</x:v>
-      </x:c>
-      <x:c r="B93" s="0" t="s">
-        <x:v>203</x:v>
       </x:c>
       <x:c r="C93" s="0" t="s">
         <x:v>5</x:v>
@@ -2346,10 +2319,10 @@
     </x:row>
     <x:row r="94" spans="1:3">
       <x:c r="A94" s="0" t="s">
+        <x:v>203</x:v>
+      </x:c>
+      <x:c r="B94" s="0" t="s">
         <x:v>204</x:v>
-      </x:c>
-      <x:c r="B94" s="0" t="s">
-        <x:v>205</x:v>
       </x:c>
       <x:c r="C94" s="0" t="s">
         <x:v>5</x:v>
@@ -2357,10 +2330,10 @@
     </x:row>
     <x:row r="95" spans="1:3">
       <x:c r="A95" s="0" t="s">
+        <x:v>205</x:v>
+      </x:c>
+      <x:c r="B95" s="0" t="s">
         <x:v>206</x:v>
-      </x:c>
-      <x:c r="B95" s="0" t="s">
-        <x:v>207</x:v>
       </x:c>
       <x:c r="C95" s="0" t="s">
         <x:v>5</x:v>
@@ -2368,10 +2341,10 @@
     </x:row>
     <x:row r="96" spans="1:3">
       <x:c r="A96" s="0" t="s">
+        <x:v>207</x:v>
+      </x:c>
+      <x:c r="B96" s="0" t="s">
         <x:v>208</x:v>
-      </x:c>
-      <x:c r="B96" s="0" t="s">
-        <x:v>209</x:v>
       </x:c>
       <x:c r="C96" s="0" t="s">
         <x:v>5</x:v>
@@ -2379,10 +2352,10 @@
     </x:row>
     <x:row r="97" spans="1:3">
       <x:c r="A97" s="0" t="s">
+        <x:v>209</x:v>
+      </x:c>
+      <x:c r="B97" s="0" t="s">
         <x:v>210</x:v>
-      </x:c>
-      <x:c r="B97" s="0" t="s">
-        <x:v>211</x:v>
       </x:c>
       <x:c r="C97" s="0" t="s">
         <x:v>5</x:v>
@@ -2390,10 +2363,10 @@
     </x:row>
     <x:row r="98" spans="1:3">
       <x:c r="A98" s="0" t="s">
+        <x:v>211</x:v>
+      </x:c>
+      <x:c r="B98" s="0" t="s">
         <x:v>212</x:v>
-      </x:c>
-      <x:c r="B98" s="0" t="s">
-        <x:v>213</x:v>
       </x:c>
       <x:c r="C98" s="0" t="s">
         <x:v>5</x:v>
@@ -2401,10 +2374,10 @@
     </x:row>
     <x:row r="99" spans="1:3">
       <x:c r="A99" s="0" t="s">
+        <x:v>213</x:v>
+      </x:c>
+      <x:c r="B99" s="0" t="s">
         <x:v>214</x:v>
-      </x:c>
-      <x:c r="B99" s="0" t="s">
-        <x:v>215</x:v>
       </x:c>
       <x:c r="C99" s="0" t="s">
         <x:v>5</x:v>
@@ -2412,10 +2385,10 @@
     </x:row>
     <x:row r="100" spans="1:3">
       <x:c r="A100" s="0" t="s">
+        <x:v>215</x:v>
+      </x:c>
+      <x:c r="B100" s="0" t="s">
         <x:v>216</x:v>
-      </x:c>
-      <x:c r="B100" s="0" t="s">
-        <x:v>217</x:v>
       </x:c>
       <x:c r="C100" s="0" t="s">
         <x:v>5</x:v>
@@ -2423,10 +2396,10 @@
     </x:row>
     <x:row r="101" spans="1:3">
       <x:c r="A101" s="0" t="s">
+        <x:v>217</x:v>
+      </x:c>
+      <x:c r="B101" s="0" t="s">
         <x:v>218</x:v>
-      </x:c>
-      <x:c r="B101" s="0" t="s">
-        <x:v>219</x:v>
       </x:c>
       <x:c r="C101" s="0" t="s">
         <x:v>5</x:v>
@@ -2434,10 +2407,10 @@
     </x:row>
     <x:row r="102" spans="1:3">
       <x:c r="A102" s="0" t="s">
+        <x:v>219</x:v>
+      </x:c>
+      <x:c r="B102" s="0" t="s">
         <x:v>220</x:v>
-      </x:c>
-      <x:c r="B102" s="0" t="s">
-        <x:v>221</x:v>
       </x:c>
       <x:c r="C102" s="0" t="s">
         <x:v>5</x:v>
@@ -2445,10 +2418,10 @@
     </x:row>
     <x:row r="103" spans="1:3">
       <x:c r="A103" s="0" t="s">
+        <x:v>221</x:v>
+      </x:c>
+      <x:c r="B103" s="0" t="s">
         <x:v>222</x:v>
-      </x:c>
-      <x:c r="B103" s="0" t="s">
-        <x:v>223</x:v>
       </x:c>
       <x:c r="C103" s="0" t="s">
         <x:v>5</x:v>
@@ -2456,10 +2429,10 @@
     </x:row>
     <x:row r="104" spans="1:3">
       <x:c r="A104" s="0" t="s">
+        <x:v>223</x:v>
+      </x:c>
+      <x:c r="B104" s="0" t="s">
         <x:v>224</x:v>
-      </x:c>
-      <x:c r="B104" s="0" t="s">
-        <x:v>225</x:v>
       </x:c>
       <x:c r="C104" s="0" t="s">
         <x:v>5</x:v>
@@ -2467,21 +2440,21 @@
     </x:row>
     <x:row r="105" spans="1:3">
       <x:c r="A105" s="0" t="s">
+        <x:v>225</x:v>
+      </x:c>
+      <x:c r="B105" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="C105" s="0" t="s">
         <x:v>226</x:v>
-      </x:c>
-      <x:c r="B105" s="0" t="s">
-        <x:v>227</x:v>
-      </x:c>
-      <x:c r="C105" s="0" t="s">
-        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="106" spans="1:3">
       <x:c r="A106" s="0" t="s">
+        <x:v>227</x:v>
+      </x:c>
+      <x:c r="B106" s="0" t="s">
         <x:v>228</x:v>
-      </x:c>
-      <x:c r="B106" s="0" t="s">
-        <x:v>229</x:v>
       </x:c>
       <x:c r="C106" s="0" t="s">
         <x:v>5</x:v>
@@ -2489,10 +2462,10 @@
     </x:row>
     <x:row r="107" spans="1:3">
       <x:c r="A107" s="0" t="s">
+        <x:v>229</x:v>
+      </x:c>
+      <x:c r="B107" s="0" t="s">
         <x:v>230</x:v>
-      </x:c>
-      <x:c r="B107" s="0" t="s">
-        <x:v>231</x:v>
       </x:c>
       <x:c r="C107" s="0" t="s">
         <x:v>5</x:v>
@@ -2500,10 +2473,10 @@
     </x:row>
     <x:row r="108" spans="1:3">
       <x:c r="A108" s="0" t="s">
+        <x:v>231</x:v>
+      </x:c>
+      <x:c r="B108" s="0" t="s">
         <x:v>232</x:v>
-      </x:c>
-      <x:c r="B108" s="0" t="s">
-        <x:v>233</x:v>
       </x:c>
       <x:c r="C108" s="0" t="s">
         <x:v>5</x:v>
@@ -2511,24 +2484,24 @@
     </x:row>
     <x:row r="109" spans="1:3">
       <x:c r="A109" s="0" t="s">
+        <x:v>233</x:v>
+      </x:c>
+      <x:c r="B109" s="0" t="s">
         <x:v>234</x:v>
       </x:c>
-      <x:c r="B109" s="0" t="s">
-        <x:v>58</x:v>
-      </x:c>
       <x:c r="C109" s="0" t="s">
-        <x:v>235</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="110" spans="1:3">
       <x:c r="A110" s="0" t="s">
+        <x:v>235</x:v>
+      </x:c>
+      <x:c r="B110" s="0" t="s">
         <x:v>236</x:v>
       </x:c>
-      <x:c r="B110" s="0" t="s">
+      <x:c r="C110" s="0" t="s">
         <x:v>237</x:v>
-      </x:c>
-      <x:c r="C110" s="0" t="s">
-        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="111" spans="1:3">
@@ -2539,7 +2512,7 @@
         <x:v>239</x:v>
       </x:c>
       <x:c r="C111" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="112" spans="1:3">
@@ -2550,37 +2523,37 @@
         <x:v>241</x:v>
       </x:c>
       <x:c r="C112" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>242</x:v>
       </x:c>
     </x:row>
     <x:row r="113" spans="1:3">
       <x:c r="A113" s="0" t="s">
-        <x:v>242</x:v>
+        <x:v>243</x:v>
       </x:c>
       <x:c r="B113" s="0" t="s">
-        <x:v>243</x:v>
+        <x:v>244</x:v>
       </x:c>
       <x:c r="C113" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>245</x:v>
       </x:c>
     </x:row>
     <x:row r="114" spans="1:3">
       <x:c r="A114" s="0" t="s">
-        <x:v>244</x:v>
+        <x:v>246</x:v>
       </x:c>
       <x:c r="B114" s="0" t="s">
-        <x:v>245</x:v>
+        <x:v>247</x:v>
       </x:c>
       <x:c r="C114" s="0" t="s">
-        <x:v>246</x:v>
+        <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="115" spans="1:3">
       <x:c r="A115" s="0" t="s">
-        <x:v>247</x:v>
+        <x:v>248</x:v>
       </x:c>
       <x:c r="B115" s="0" t="s">
-        <x:v>248</x:v>
+        <x:v>249</x:v>
       </x:c>
       <x:c r="C115" s="0" t="s">
         <x:v>58</x:v>
@@ -2588,13 +2561,13 @@
     </x:row>
     <x:row r="116" spans="1:3">
       <x:c r="A116" s="0" t="s">
-        <x:v>249</x:v>
+        <x:v>250</x:v>
       </x:c>
       <x:c r="B116" s="0" t="s">
-        <x:v>250</x:v>
+        <x:v>251</x:v>
       </x:c>
       <x:c r="C116" s="0" t="s">
-        <x:v>251</x:v>
+        <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="117" spans="1:3">
@@ -2605,18 +2578,18 @@
         <x:v>253</x:v>
       </x:c>
       <x:c r="C117" s="0" t="s">
-        <x:v>254</x:v>
+        <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="118" spans="1:3">
       <x:c r="A118" s="0" t="s">
+        <x:v>254</x:v>
+      </x:c>
+      <x:c r="B118" s="0" t="s">
         <x:v>255</x:v>
       </x:c>
-      <x:c r="B118" s="0" t="s">
+      <x:c r="C118" s="0" t="s">
         <x:v>256</x:v>
-      </x:c>
-      <x:c r="C118" s="0" t="s">
-        <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="119" spans="1:3">
@@ -2627,15 +2600,15 @@
         <x:v>258</x:v>
       </x:c>
       <x:c r="C119" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>259</x:v>
       </x:c>
     </x:row>
     <x:row r="120" spans="1:3">
       <x:c r="A120" s="0" t="s">
-        <x:v>259</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="B120" s="0" t="s">
-        <x:v>260</x:v>
+        <x:v>261</x:v>
       </x:c>
       <x:c r="C120" s="0" t="s">
         <x:v>58</x:v>
@@ -2643,43 +2616,43 @@
     </x:row>
     <x:row r="121" spans="1:3">
       <x:c r="A121" s="0" t="s">
-        <x:v>261</x:v>
+        <x:v>262</x:v>
       </x:c>
       <x:c r="B121" s="0" t="s">
-        <x:v>262</x:v>
+        <x:v>263</x:v>
       </x:c>
       <x:c r="C121" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>264</x:v>
       </x:c>
     </x:row>
     <x:row r="122" spans="1:3">
       <x:c r="A122" s="0" t="s">
-        <x:v>263</x:v>
+        <x:v>265</x:v>
       </x:c>
       <x:c r="B122" s="0" t="s">
-        <x:v>264</x:v>
+        <x:v>266</x:v>
       </x:c>
       <x:c r="C122" s="0" t="s">
-        <x:v>265</x:v>
+        <x:v>267</x:v>
       </x:c>
     </x:row>
     <x:row r="123" spans="1:3">
       <x:c r="A123" s="0" t="s">
-        <x:v>266</x:v>
+        <x:v>268</x:v>
       </x:c>
       <x:c r="B123" s="0" t="s">
-        <x:v>267</x:v>
+        <x:v>269</x:v>
       </x:c>
       <x:c r="C123" s="0" t="s">
-        <x:v>268</x:v>
+        <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="124" spans="1:3">
       <x:c r="A124" s="0" t="s">
-        <x:v>269</x:v>
+        <x:v>270</x:v>
       </x:c>
       <x:c r="B124" s="0" t="s">
-        <x:v>270</x:v>
+        <x:v>271</x:v>
       </x:c>
       <x:c r="C124" s="0" t="s">
         <x:v>58</x:v>
@@ -2687,13 +2660,13 @@
     </x:row>
     <x:row r="125" spans="1:3">
       <x:c r="A125" s="0" t="s">
-        <x:v>271</x:v>
+        <x:v>272</x:v>
       </x:c>
       <x:c r="B125" s="0" t="s">
-        <x:v>272</x:v>
+        <x:v>273</x:v>
       </x:c>
       <x:c r="C125" s="0" t="s">
-        <x:v>273</x:v>
+        <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="126" spans="1:3">
@@ -2704,15 +2677,15 @@
         <x:v>275</x:v>
       </x:c>
       <x:c r="C126" s="0" t="s">
-        <x:v>276</x:v>
+        <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="127" spans="1:3">
       <x:c r="A127" s="0" t="s">
+        <x:v>276</x:v>
+      </x:c>
+      <x:c r="B127" s="0" t="s">
         <x:v>277</x:v>
-      </x:c>
-      <x:c r="B127" s="0" t="s">
-        <x:v>278</x:v>
       </x:c>
       <x:c r="C127" s="0" t="s">
         <x:v>58</x:v>
@@ -2720,10 +2693,10 @@
     </x:row>
     <x:row r="128" spans="1:3">
       <x:c r="A128" s="0" t="s">
+        <x:v>278</x:v>
+      </x:c>
+      <x:c r="B128" s="0" t="s">
         <x:v>279</x:v>
-      </x:c>
-      <x:c r="B128" s="0" t="s">
-        <x:v>280</x:v>
       </x:c>
       <x:c r="C128" s="0" t="s">
         <x:v>58</x:v>
@@ -2731,32 +2704,32 @@
     </x:row>
     <x:row r="129" spans="1:3">
       <x:c r="A129" s="0" t="s">
+        <x:v>280</x:v>
+      </x:c>
+      <x:c r="B129" s="0" t="s">
         <x:v>281</x:v>
       </x:c>
-      <x:c r="B129" s="0" t="s">
-        <x:v>282</x:v>
-      </x:c>
       <x:c r="C129" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="130" spans="1:3">
       <x:c r="A130" s="0" t="s">
+        <x:v>282</x:v>
+      </x:c>
+      <x:c r="B130" s="0" t="s">
         <x:v>283</x:v>
       </x:c>
-      <x:c r="B130" s="0" t="s">
-        <x:v>284</x:v>
-      </x:c>
       <x:c r="C130" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="131" spans="1:3">
       <x:c r="A131" s="0" t="s">
+        <x:v>284</x:v>
+      </x:c>
+      <x:c r="B131" s="0" t="s">
         <x:v>285</x:v>
-      </x:c>
-      <x:c r="B131" s="0" t="s">
-        <x:v>286</x:v>
       </x:c>
       <x:c r="C131" s="0" t="s">
         <x:v>58</x:v>
@@ -2764,10 +2737,10 @@
     </x:row>
     <x:row r="132" spans="1:3">
       <x:c r="A132" s="0" t="s">
+        <x:v>286</x:v>
+      </x:c>
+      <x:c r="B132" s="0" t="s">
         <x:v>287</x:v>
-      </x:c>
-      <x:c r="B132" s="0" t="s">
-        <x:v>288</x:v>
       </x:c>
       <x:c r="C132" s="0" t="s">
         <x:v>58</x:v>
@@ -2775,32 +2748,32 @@
     </x:row>
     <x:row r="133" spans="1:3">
       <x:c r="A133" s="0" t="s">
+        <x:v>288</x:v>
+      </x:c>
+      <x:c r="B133" s="0" t="s">
         <x:v>289</x:v>
       </x:c>
-      <x:c r="B133" s="0" t="s">
-        <x:v>290</x:v>
-      </x:c>
       <x:c r="C133" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="134" spans="1:3">
       <x:c r="A134" s="0" t="s">
+        <x:v>290</x:v>
+      </x:c>
+      <x:c r="B134" s="0" t="s">
         <x:v>291</x:v>
       </x:c>
-      <x:c r="B134" s="0" t="s">
-        <x:v>292</x:v>
-      </x:c>
       <x:c r="C134" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="135" spans="1:3">
       <x:c r="A135" s="0" t="s">
+        <x:v>292</x:v>
+      </x:c>
+      <x:c r="B135" s="0" t="s">
         <x:v>293</x:v>
-      </x:c>
-      <x:c r="B135" s="0" t="s">
-        <x:v>294</x:v>
       </x:c>
       <x:c r="C135" s="0" t="s">
         <x:v>58</x:v>
@@ -2808,10 +2781,10 @@
     </x:row>
     <x:row r="136" spans="1:3">
       <x:c r="A136" s="0" t="s">
+        <x:v>294</x:v>
+      </x:c>
+      <x:c r="B136" s="0" t="s">
         <x:v>295</x:v>
-      </x:c>
-      <x:c r="B136" s="0" t="s">
-        <x:v>296</x:v>
       </x:c>
       <x:c r="C136" s="0" t="s">
         <x:v>58</x:v>
@@ -2819,10 +2792,10 @@
     </x:row>
     <x:row r="137" spans="1:3">
       <x:c r="A137" s="0" t="s">
+        <x:v>296</x:v>
+      </x:c>
+      <x:c r="B137" s="0" t="s">
         <x:v>297</x:v>
-      </x:c>
-      <x:c r="B137" s="0" t="s">
-        <x:v>298</x:v>
       </x:c>
       <x:c r="C137" s="0" t="s">
         <x:v>58</x:v>
@@ -2830,10 +2803,10 @@
     </x:row>
     <x:row r="138" spans="1:3">
       <x:c r="A138" s="0" t="s">
+        <x:v>298</x:v>
+      </x:c>
+      <x:c r="B138" s="0" t="s">
         <x:v>299</x:v>
-      </x:c>
-      <x:c r="B138" s="0" t="s">
-        <x:v>300</x:v>
       </x:c>
       <x:c r="C138" s="0" t="s">
         <x:v>58</x:v>
@@ -2841,10 +2814,10 @@
     </x:row>
     <x:row r="139" spans="1:3">
       <x:c r="A139" s="0" t="s">
+        <x:v>300</x:v>
+      </x:c>
+      <x:c r="B139" s="0" t="s">
         <x:v>301</x:v>
-      </x:c>
-      <x:c r="B139" s="0" t="s">
-        <x:v>302</x:v>
       </x:c>
       <x:c r="C139" s="0" t="s">
         <x:v>58</x:v>
@@ -2852,10 +2825,10 @@
     </x:row>
     <x:row r="140" spans="1:3">
       <x:c r="A140" s="0" t="s">
+        <x:v>302</x:v>
+      </x:c>
+      <x:c r="B140" s="0" t="s">
         <x:v>303</x:v>
-      </x:c>
-      <x:c r="B140" s="0" t="s">
-        <x:v>304</x:v>
       </x:c>
       <x:c r="C140" s="0" t="s">
         <x:v>58</x:v>
@@ -2863,10 +2836,10 @@
     </x:row>
     <x:row r="141" spans="1:3">
       <x:c r="A141" s="0" t="s">
+        <x:v>304</x:v>
+      </x:c>
+      <x:c r="B141" s="0" t="s">
         <x:v>305</x:v>
-      </x:c>
-      <x:c r="B141" s="0" t="s">
-        <x:v>306</x:v>
       </x:c>
       <x:c r="C141" s="0" t="s">
         <x:v>58</x:v>
@@ -2874,10 +2847,10 @@
     </x:row>
     <x:row r="142" spans="1:3">
       <x:c r="A142" s="0" t="s">
+        <x:v>306</x:v>
+      </x:c>
+      <x:c r="B142" s="0" t="s">
         <x:v>307</x:v>
-      </x:c>
-      <x:c r="B142" s="0" t="s">
-        <x:v>308</x:v>
       </x:c>
       <x:c r="C142" s="0" t="s">
         <x:v>58</x:v>
@@ -2885,10 +2858,10 @@
     </x:row>
     <x:row r="143" spans="1:3">
       <x:c r="A143" s="0" t="s">
-        <x:v>309</x:v>
+        <x:v>300</x:v>
       </x:c>
       <x:c r="B143" s="0" t="s">
-        <x:v>310</x:v>
+        <x:v>301</x:v>
       </x:c>
       <x:c r="C143" s="0" t="s">
         <x:v>58</x:v>
@@ -2896,10 +2869,10 @@
     </x:row>
     <x:row r="144" spans="1:3">
       <x:c r="A144" s="0" t="s">
-        <x:v>311</x:v>
+        <x:v>302</x:v>
       </x:c>
       <x:c r="B144" s="0" t="s">
-        <x:v>312</x:v>
+        <x:v>303</x:v>
       </x:c>
       <x:c r="C144" s="0" t="s">
         <x:v>58</x:v>
@@ -2907,10 +2880,10 @@
     </x:row>
     <x:row r="145" spans="1:3">
       <x:c r="A145" s="0" t="s">
-        <x:v>313</x:v>
+        <x:v>304</x:v>
       </x:c>
       <x:c r="B145" s="0" t="s">
-        <x:v>314</x:v>
+        <x:v>305</x:v>
       </x:c>
       <x:c r="C145" s="0" t="s">
         <x:v>58</x:v>
@@ -2918,10 +2891,10 @@
     </x:row>
     <x:row r="146" spans="1:3">
       <x:c r="A146" s="0" t="s">
-        <x:v>315</x:v>
+        <x:v>306</x:v>
       </x:c>
       <x:c r="B146" s="0" t="s">
-        <x:v>316</x:v>
+        <x:v>307</x:v>
       </x:c>
       <x:c r="C146" s="0" t="s">
         <x:v>58</x:v>
@@ -2929,10 +2902,10 @@
     </x:row>
     <x:row r="147" spans="1:3">
       <x:c r="A147" s="0" t="s">
-        <x:v>315</x:v>
+        <x:v>306</x:v>
       </x:c>
       <x:c r="B147" s="0" t="s">
-        <x:v>316</x:v>
+        <x:v>307</x:v>
       </x:c>
       <x:c r="C147" s="0" t="s">
         <x:v>58</x:v>

</xml_diff>

<commit_message>
Added Exclusion according to the tabs and login updated
</commit_message>
<xml_diff>
--- a/Inputs/New Microsoft Excel Worksheet.xlsx
+++ b/Inputs/New Microsoft Excel Worksheet.xlsx
@@ -25,15 +25,186 @@
     <x:t>SmallBox DD WEB ID</x:t>
   </x:si>
   <x:si>
+    <x:t>Zinger® Burger</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32879</x:t>
+  </x:si>
+  <x:si>
+    <x:t>same</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Zinger® Burger Combo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32880</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Double Tender™ Burger</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32886</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Zinger® Bacon &amp; Cheese Burger</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32887</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Zinger® Crunch Burger™</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32888</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Original Crispy Burger</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32889</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Original Crispy Bacon &amp; Cheese Burger</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32890</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Original Crispy BBQ Bacon Stacker® Burger</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32891</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Zinger Stacker® Burger</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32892</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Original Pepper Mayo Slider</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32897</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Original BBQ Slider</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32898</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Original Crunch Twister® </x:t>
+  </x:si>
+  <x:si>
+    <x:t>32899</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Zinger® Crunch Twister®  </x:t>
+  </x:si>
+  <x:si>
+    <x:t>32900</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Original Supercharged Slider </x:t>
+  </x:si>
+  <x:si>
+    <x:t>32901</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Regular Potato &amp; Gravy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32904</x:t>
+  </x:si>
+  <x:si>
+    <x:t>n/a</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Large Potato &amp; Gravy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32905</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Regular Coleslaw</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32906</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Large Coleslaw</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32907</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Regular Gravy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32908</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Crunchy Jalapeno Slaw</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32909</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Dinner Roll</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32910</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Double Chocolate Mousse</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32911</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Original Tenders™ Crunch Bowl</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32912</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Zinger® Crunch Bowl</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32913</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Go Bucket® 2 Wicked Wings®</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32914</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Go Bucket® 1 Original Tender™</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32915</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Go Bucket® Popcorn Chicken®</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32916</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Go Bucket® 3 Nuggets</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32917</x:t>
+  </x:si>
+  <x:si>
     <x:t>1 Piece of Chicken</x:t>
   </x:si>
   <x:si>
     <x:t>32922</x:t>
   </x:si>
   <x:si>
-    <x:t>same</x:t>
-  </x:si>
-  <x:si>
     <x:t>6 Pieces of Chicken</x:t>
   </x:si>
   <x:si>
@@ -46,6 +217,30 @@
     <x:t>32924</x:t>
   </x:si>
   <x:si>
+    <x:t>3 Wicked Wings®</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32925</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6 Wicked Wings®</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32926</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10 Wicked Wings®</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32927</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Zinger® Fillet Piece</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32928</x:t>
+  </x:si>
+  <x:si>
     <x:t>Original Crispy Fillet Piece</x:t>
   </x:si>
   <x:si>
@@ -64,6 +259,168 @@
     <x:t>32931</x:t>
   </x:si>
   <x:si>
+    <x:t>3 Original Tenders™</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32932</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5 Original Tenders™</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32933</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6 Nuggets</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32934</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10 Nuggets</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32935</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Regular Popcorn Chicken®</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32936</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Maxi Popcorn Chicken®</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32937</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Snack Popcorn Chicken®</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32938</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Double Tender™ Burger Combo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32939</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Zinger Stacker® Burger Combo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32940</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Original Crispy Burger Combo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32941</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Zinger® Crunch Burger™ Combo </x:t>
+  </x:si>
+  <x:si>
+    <x:t>32942</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Original Crispy Bacon &amp; Cheese Burger Combo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32943</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Original Crispy BBQ Bacon Stacker® Burger Combo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32944</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Zinger® Bacon &amp; Cheese Burger Combo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32945</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Original Crunch Twister® Combo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32946</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Zinger® Crunch Twister® Combo </x:t>
+  </x:si>
+  <x:si>
+    <x:t>32947</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Zinger® Crunch Bowl Combo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32948</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Original Tenders™ Crunch Bowl Combo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32949</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kids Meal with BBQ Slider</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32950</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kids Meal with Nuggets</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32951</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kids Meal with Snack Popcorn Chicken®</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32952</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Regular Popcorn Chicken® Combo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32954</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Maxi Popcorn Chicken® Combo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32955</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6 Wicked Wings® Combo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32956</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Snack Popcorn Chicken® Combo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32957</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10 Wicked Wings® Combo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32958</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3 Wicked Wings® Combo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32959</x:t>
+  </x:si>
+  <x:si>
     <x:t xml:space="preserve">3 Pieces Combo Hot &amp; Crispy™ </x:t>
   </x:si>
   <x:si>
@@ -76,6 +433,30 @@
     <x:t>32961</x:t>
   </x:si>
   <x:si>
+    <x:t>6 Nugget Combo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32962</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10 Nugget Combo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32963</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3 Original Tenders™ Combo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32964</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5 Original Tenders™ Combo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32965</x:t>
+  </x:si>
+  <x:si>
     <x:t>Zinger® Burger Box Hot &amp; Crispy™</x:t>
   </x:si>
   <x:si>
@@ -190,9 +571,6 @@
     <x:t>32978</x:t>
   </x:si>
   <x:si>
-    <x:t>n/a</x:t>
-  </x:si>
-  <x:si>
     <x:t>Burger Feast</x:t>
   </x:si>
   <x:si>
@@ -256,6 +634,102 @@
     <x:t>33215</x:t>
   </x:si>
   <x:si>
+    <x:t>Go Bucket® Hot &amp; Crispy™</x:t>
+  </x:si>
+  <x:si>
+    <x:t>33216</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4 Dipping Sauces</x:t>
+  </x:si>
+  <x:si>
+    <x:t>33218</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Bottled Water</x:t>
+  </x:si>
+  <x:si>
+    <x:t>33219</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sparkling Water</x:t>
+  </x:si>
+  <x:si>
+    <x:t>33220</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Apple Juice</x:t>
+  </x:si>
+  <x:si>
+    <x:t>33221</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Lipton Peach Ice Tea</x:t>
+  </x:si>
+  <x:si>
+    <x:t>33222</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Spicy Mango Lemonade~</x:t>
+  </x:si>
+  <x:si>
+    <x:t>33223</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sparkling Raspberry Lemonade~</x:t>
+  </x:si>
+  <x:si>
+    <x:t>33224</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Iced Latte</x:t>
+  </x:si>
+  <x:si>
+    <x:t>33225</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Watermelon Boba Refresher~</x:t>
+  </x:si>
+  <x:si>
+    <x:t>33226</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Cherry Boba Refresher~</x:t>
+  </x:si>
+  <x:si>
+    <x:t>33227</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Caramel Krunch Shake</x:t>
+  </x:si>
+  <x:si>
+    <x:t>33228</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Chocolate Krunch Shake</x:t>
+  </x:si>
+  <x:si>
+    <x:t>33229</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Coconut Mango Krunch Shake</x:t>
+  </x:si>
+  <x:si>
+    <x:t>33230</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Iced Mocha Koffee Krunch</x:t>
+  </x:si>
+  <x:si>
+    <x:t>33231</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Iced Caramel Koffee Krunch</x:t>
+  </x:si>
+  <x:si>
+    <x:t>33232</x:t>
+  </x:si>
+  <x:si>
     <x:t>33006</x:t>
   </x:si>
   <x:si>
@@ -277,495 +751,12 @@
     <x:t>33213</x:t>
   </x:si>
   <x:si>
-    <x:t>Zinger® Burger</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32879</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Zinger® Burger Combo</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32880</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Double Tender™ Burger</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32886</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Zinger® Bacon &amp; Cheese Burger</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32887</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Zinger® Crunch Burger™</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32888</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Original Crispy Burger</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32889</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Original Crispy Bacon &amp; Cheese Burger</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32890</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Original Crispy BBQ Bacon Stacker® Burger</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32891</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Zinger Stacker® Burger</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32892</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3 Wicked Wings®</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32925</x:t>
-  </x:si>
-  <x:si>
-    <x:t>6 Wicked Wings®</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32926</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10 Wicked Wings®</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32927</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Zinger® Fillet Piece</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32928</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3 Original Tenders™</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32932</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5 Original Tenders™</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32933</x:t>
-  </x:si>
-  <x:si>
-    <x:t>6 Nuggets</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32934</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10 Nuggets</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32935</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Regular Popcorn Chicken®</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32936</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Maxi Popcorn Chicken®</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32937</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Snack Popcorn Chicken®</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32938</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Double Tender™ Burger Combo</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32939</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Zinger Stacker® Burger Combo</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32940</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Original Crispy Burger Combo</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32941</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Original Crispy Bacon &amp; Cheese Burger Combo</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32943</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Original Crispy BBQ Bacon Stacker® Burger Combo</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32944</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Zinger® Bacon &amp; Cheese Burger Combo</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32945</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Regular Popcorn Chicken® Combo</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32954</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Maxi Popcorn Chicken® Combo</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32955</x:t>
-  </x:si>
-  <x:si>
-    <x:t>6 Wicked Wings® Combo</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32956</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Snack Popcorn Chicken® Combo</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32957</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10 Wicked Wings® Combo</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32958</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3 Wicked Wings® Combo</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32959</x:t>
-  </x:si>
-  <x:si>
-    <x:t>6 Nugget Combo</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32962</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10 Nugget Combo</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32963</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3 Original Tenders™ Combo</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32964</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5 Original Tenders™ Combo</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32965</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Original Pepper Mayo Slider</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32897</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Original BBQ Slider</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32898</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Original Crunch Twister® </x:t>
-  </x:si>
-  <x:si>
-    <x:t>32899</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Zinger® Crunch Twister®  </x:t>
-  </x:si>
-  <x:si>
-    <x:t>32900</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Original Supercharged Slider </x:t>
-  </x:si>
-  <x:si>
-    <x:t>32901</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Regular Potato &amp; Gravy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32904</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Large Potato &amp; Gravy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32905</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Regular Coleslaw</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32906</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Large Coleslaw</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32907</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Regular Gravy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32908</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Crunchy Jalapeno Slaw</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32909</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Dinner Roll</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32910</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Double Chocolate Mousse</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32911</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Original Tenders™ Crunch Bowl</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32912</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Zinger® Crunch Bowl</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32913</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Go Bucket® 2 Wicked Wings®</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32914</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Go Bucket® 1 Original Tender™</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32915</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Go Bucket® Popcorn Chicken®</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32916</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Go Bucket® 3 Nuggets</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32917</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Zinger® Crunch Burger™ Combo </x:t>
-  </x:si>
-  <x:si>
-    <x:t>32942</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Original Crunch Twister® Combo</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32946</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Zinger® Crunch Twister® Combo </x:t>
-  </x:si>
-  <x:si>
-    <x:t>32947</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Zinger® Crunch Bowl Combo</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32948</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Original Tenders™ Crunch Bowl Combo</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32949</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kids Meal with BBQ Slider</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32950</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kids Meal with Nuggets</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32951</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kids Meal with Snack Popcorn Chicken®</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32952</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Go Bucket® Hot &amp; Crispy™</x:t>
-  </x:si>
-  <x:si>
-    <x:t>33216</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4 Dipping Sauces</x:t>
-  </x:si>
-  <x:si>
-    <x:t>33218</x:t>
-  </x:si>
-  <x:si>
-    <x:t>BBQ Dip</x:t>
-  </x:si>
-  <x:si>
-    <x:t>43819</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Supercharged Dip</x:t>
-  </x:si>
-  <x:si>
-    <x:t>43820</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Aioli Dip</x:t>
-  </x:si>
-  <x:si>
-    <x:t>43823</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Jalapeno Mayo Dip</x:t>
-  </x:si>
-  <x:si>
-    <x:t>44003</x:t>
-  </x:si>
-  <x:si>
     <x:t>Large Coleslaw(4x110g)</x:t>
   </x:si>
   <x:si>
     <x:t>33217</x:t>
   </x:si>
   <x:si>
-    <x:t>Sweet &amp; Sour Dip</x:t>
-  </x:si>
-  <x:si>
-    <x:t>43822</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sweet Chilli Dip</x:t>
-  </x:si>
-  <x:si>
-    <x:t>43821</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Tomato Dip</x:t>
-  </x:si>
-  <x:si>
-    <x:t>43810</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Regular Pepsi Max^</x:t>
-  </x:si>
-  <x:si>
-    <x:t>43829</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Large Pepsi Max^</x:t>
-  </x:si>
-  <x:si>
-    <x:t>43830</x:t>
-  </x:si>
-  <x:si>
-    <x:t>43848</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.25L Pepsi Max^</x:t>
-  </x:si>
-  <x:si>
-    <x:t>43831</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Regular Pepsi^</x:t>
-  </x:si>
-  <x:si>
-    <x:t>43811</x:t>
-  </x:si>
-  <x:si>
-    <x:t>43849</x:t>
-  </x:si>
-  <x:si>
-    <x:t>LargePepsi^</x:t>
-  </x:si>
-  <x:si>
-    <x:t>43827</x:t>
-  </x:si>
-  <x:si>
-    <x:t>43850</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.25L Pepsi^</x:t>
-  </x:si>
-  <x:si>
-    <x:t>43828</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Regular 7Up</x:t>
-  </x:si>
-  <x:si>
-    <x:t>43832</x:t>
-  </x:si>
-  <x:si>
     <x:t>Large 7Up</x:t>
   </x:si>
   <x:si>
@@ -854,90 +845,6 @@
   </x:si>
   <x:si>
     <x:t>43846</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Bottled Water</x:t>
-  </x:si>
-  <x:si>
-    <x:t>33219</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sparkling Water</x:t>
-  </x:si>
-  <x:si>
-    <x:t>33220</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Apple Juice</x:t>
-  </x:si>
-  <x:si>
-    <x:t>33221</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Lipton Peach Ice Tea</x:t>
-  </x:si>
-  <x:si>
-    <x:t>33222</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Iced Mocha Koffee Krunch</x:t>
-  </x:si>
-  <x:si>
-    <x:t>33231</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Iced Caramel Koffee Krunch</x:t>
-  </x:si>
-  <x:si>
-    <x:t>33232</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Iced Latte</x:t>
-  </x:si>
-  <x:si>
-    <x:t>33225</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Watermelon Boba Refresher~</x:t>
-  </x:si>
-  <x:si>
-    <x:t>33226</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Cherry Boba Refresher~</x:t>
-  </x:si>
-  <x:si>
-    <x:t>33227</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Chocolate Krunch Shake</x:t>
-  </x:si>
-  <x:si>
-    <x:t>33229</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Caramel Krunch Shake</x:t>
-  </x:si>
-  <x:si>
-    <x:t>33228</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Coconut Mango Krunch Shake</x:t>
-  </x:si>
-  <x:si>
-    <x:t>33230</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sparkling Raspberry Lemonade~</x:t>
-  </x:si>
-  <x:si>
-    <x:t>33224</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Spicy Mango Lemonade~</x:t>
-  </x:si>
-  <x:si>
-    <x:t>33223</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -1401,169 +1308,169 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:3">
       <x:c r="A11" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="B11" s="0" t="s">
-        <x:v>24</x:v>
-      </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:3">
       <x:c r="A12" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:3">
       <x:c r="A13" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="C13" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:3">
       <x:c r="A14" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="C14" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:3">
       <x:c r="A15" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C15" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:3">
       <x:c r="A16" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="C16" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:3">
       <x:c r="A17" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="C17" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:3">
       <x:c r="A18" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C18" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:3">
       <x:c r="A19" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="C19" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:3">
       <x:c r="A20" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="C20" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:3">
       <x:c r="A21" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="C21" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:3">
       <x:c r="A22" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="C22" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:3">
       <x:c r="A23" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="C23" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:3">
       <x:c r="A24" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="C24" s="0" t="s">
-        <x:v>64</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:3">
       <x:c r="A25" s="0" t="s">
-        <x:v>65</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>66</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="C25" s="0" t="s">
         <x:v>5</x:v>
@@ -1571,32 +1478,32 @@
     </x:row>
     <x:row r="26" spans="1:3">
       <x:c r="A26" s="0" t="s">
-        <x:v>67</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="C26" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:3">
       <x:c r="A27" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
-        <x:v>70</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="C27" s="0" t="s">
-        <x:v>71</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:3">
       <x:c r="A28" s="0" t="s">
-        <x:v>72</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
-        <x:v>73</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="C28" s="0" t="s">
         <x:v>5</x:v>
@@ -1604,21 +1511,21 @@
     </x:row>
     <x:row r="29" spans="1:3">
       <x:c r="A29" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
-        <x:v>75</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="C29" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:3">
       <x:c r="A30" s="0" t="s">
-        <x:v>76</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
-        <x:v>77</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="C30" s="0" t="s">
         <x:v>5</x:v>
@@ -1626,10 +1533,10 @@
     </x:row>
     <x:row r="31" spans="1:3">
       <x:c r="A31" s="0" t="s">
-        <x:v>78</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
-        <x:v>79</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="C31" s="0" t="s">
         <x:v>5</x:v>
@@ -1637,54 +1544,54 @@
     </x:row>
     <x:row r="32" spans="1:3">
       <x:c r="A32" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="C32" s="0" t="s">
-        <x:v>80</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:3">
       <x:c r="A33" s="0" t="s">
-        <x:v>81</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="C33" s="0" t="s">
-        <x:v>82</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:3">
       <x:c r="A34" s="0" t="s">
-        <x:v>83</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="C34" s="0" t="s">
-        <x:v>84</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:3">
       <x:c r="A35" s="0" t="s">
-        <x:v>85</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="B35" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="C35" s="0" t="s">
-        <x:v>86</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:3">
       <x:c r="A36" s="0" t="s">
-        <x:v>87</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="B36" s="0" t="s">
-        <x:v>88</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="C36" s="0" t="s">
         <x:v>5</x:v>
@@ -1692,10 +1599,10 @@
     </x:row>
     <x:row r="37" spans="1:3">
       <x:c r="A37" s="0" t="s">
-        <x:v>89</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="B37" s="0" t="s">
-        <x:v>90</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="C37" s="0" t="s">
         <x:v>5</x:v>
@@ -1703,10 +1610,10 @@
     </x:row>
     <x:row r="38" spans="1:3">
       <x:c r="A38" s="0" t="s">
-        <x:v>91</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="B38" s="0" t="s">
-        <x:v>92</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="C38" s="0" t="s">
         <x:v>5</x:v>
@@ -1714,10 +1621,10 @@
     </x:row>
     <x:row r="39" spans="1:3">
       <x:c r="A39" s="0" t="s">
-        <x:v>93</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="B39" s="0" t="s">
-        <x:v>94</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="C39" s="0" t="s">
         <x:v>5</x:v>
@@ -1725,10 +1632,10 @@
     </x:row>
     <x:row r="40" spans="1:3">
       <x:c r="A40" s="0" t="s">
-        <x:v>95</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="B40" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="C40" s="0" t="s">
         <x:v>5</x:v>
@@ -1736,10 +1643,10 @@
     </x:row>
     <x:row r="41" spans="1:3">
       <x:c r="A41" s="0" t="s">
-        <x:v>97</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="B41" s="0" t="s">
-        <x:v>98</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="C41" s="0" t="s">
         <x:v>5</x:v>
@@ -1747,10 +1654,10 @@
     </x:row>
     <x:row r="42" spans="1:3">
       <x:c r="A42" s="0" t="s">
-        <x:v>99</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="B42" s="0" t="s">
-        <x:v>100</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="C42" s="0" t="s">
         <x:v>5</x:v>
@@ -1758,10 +1665,10 @@
     </x:row>
     <x:row r="43" spans="1:3">
       <x:c r="A43" s="0" t="s">
-        <x:v>101</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="B43" s="0" t="s">
-        <x:v>102</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="C43" s="0" t="s">
         <x:v>5</x:v>
@@ -1769,10 +1676,10 @@
     </x:row>
     <x:row r="44" spans="1:3">
       <x:c r="A44" s="0" t="s">
-        <x:v>103</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="B44" s="0" t="s">
-        <x:v>104</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="C44" s="0" t="s">
         <x:v>5</x:v>
@@ -1780,10 +1687,10 @@
     </x:row>
     <x:row r="45" spans="1:3">
       <x:c r="A45" s="0" t="s">
-        <x:v>105</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="B45" s="0" t="s">
-        <x:v>106</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="C45" s="0" t="s">
         <x:v>5</x:v>
@@ -1791,10 +1698,10 @@
     </x:row>
     <x:row r="46" spans="1:3">
       <x:c r="A46" s="0" t="s">
-        <x:v>107</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="B46" s="0" t="s">
-        <x:v>108</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="C46" s="0" t="s">
         <x:v>5</x:v>
@@ -1802,10 +1709,10 @@
     </x:row>
     <x:row r="47" spans="1:3">
       <x:c r="A47" s="0" t="s">
-        <x:v>109</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="B47" s="0" t="s">
-        <x:v>110</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="C47" s="0" t="s">
         <x:v>5</x:v>
@@ -1813,10 +1720,10 @@
     </x:row>
     <x:row r="48" spans="1:3">
       <x:c r="A48" s="0" t="s">
-        <x:v>111</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="B48" s="0" t="s">
-        <x:v>112</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="C48" s="0" t="s">
         <x:v>5</x:v>
@@ -1824,10 +1731,10 @@
     </x:row>
     <x:row r="49" spans="1:3">
       <x:c r="A49" s="0" t="s">
-        <x:v>113</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="B49" s="0" t="s">
-        <x:v>114</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="C49" s="0" t="s">
         <x:v>5</x:v>
@@ -1835,10 +1742,10 @@
     </x:row>
     <x:row r="50" spans="1:3">
       <x:c r="A50" s="0" t="s">
-        <x:v>115</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="B50" s="0" t="s">
-        <x:v>116</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="C50" s="0" t="s">
         <x:v>5</x:v>
@@ -1846,10 +1753,10 @@
     </x:row>
     <x:row r="51" spans="1:3">
       <x:c r="A51" s="0" t="s">
-        <x:v>117</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="B51" s="0" t="s">
-        <x:v>118</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="C51" s="0" t="s">
         <x:v>5</x:v>
@@ -1857,10 +1764,10 @@
     </x:row>
     <x:row r="52" spans="1:3">
       <x:c r="A52" s="0" t="s">
-        <x:v>119</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="B52" s="0" t="s">
-        <x:v>120</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="C52" s="0" t="s">
         <x:v>5</x:v>
@@ -1868,10 +1775,10 @@
     </x:row>
     <x:row r="53" spans="1:3">
       <x:c r="A53" s="0" t="s">
-        <x:v>121</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="B53" s="0" t="s">
-        <x:v>122</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="C53" s="0" t="s">
         <x:v>5</x:v>
@@ -1879,10 +1786,10 @@
     </x:row>
     <x:row r="54" spans="1:3">
       <x:c r="A54" s="0" t="s">
-        <x:v>123</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="B54" s="0" t="s">
-        <x:v>124</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="C54" s="0" t="s">
         <x:v>5</x:v>
@@ -1890,10 +1797,10 @@
     </x:row>
     <x:row r="55" spans="1:3">
       <x:c r="A55" s="0" t="s">
-        <x:v>125</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="B55" s="0" t="s">
-        <x:v>126</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="C55" s="0" t="s">
         <x:v>5</x:v>
@@ -1901,10 +1808,10 @@
     </x:row>
     <x:row r="56" spans="1:3">
       <x:c r="A56" s="0" t="s">
-        <x:v>127</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="B56" s="0" t="s">
-        <x:v>128</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="C56" s="0" t="s">
         <x:v>5</x:v>
@@ -1912,10 +1819,10 @@
     </x:row>
     <x:row r="57" spans="1:3">
       <x:c r="A57" s="0" t="s">
-        <x:v>129</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="B57" s="0" t="s">
-        <x:v>130</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="C57" s="0" t="s">
         <x:v>5</x:v>
@@ -1923,10 +1830,10 @@
     </x:row>
     <x:row r="58" spans="1:3">
       <x:c r="A58" s="0" t="s">
-        <x:v>131</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="B58" s="0" t="s">
-        <x:v>132</x:v>
+        <x:v>118</x:v>
       </x:c>
       <x:c r="C58" s="0" t="s">
         <x:v>5</x:v>
@@ -1934,10 +1841,10 @@
     </x:row>
     <x:row r="59" spans="1:3">
       <x:c r="A59" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="B59" s="0" t="s">
-        <x:v>134</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="C59" s="0" t="s">
         <x:v>5</x:v>
@@ -1945,10 +1852,10 @@
     </x:row>
     <x:row r="60" spans="1:3">
       <x:c r="A60" s="0" t="s">
-        <x:v>135</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="B60" s="0" t="s">
-        <x:v>136</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="C60" s="0" t="s">
         <x:v>5</x:v>
@@ -1956,10 +1863,10 @@
     </x:row>
     <x:row r="61" spans="1:3">
       <x:c r="A61" s="0" t="s">
-        <x:v>137</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="B61" s="0" t="s">
-        <x:v>138</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="C61" s="0" t="s">
         <x:v>5</x:v>
@@ -1967,10 +1874,10 @@
     </x:row>
     <x:row r="62" spans="1:3">
       <x:c r="A62" s="0" t="s">
-        <x:v>139</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="B62" s="0" t="s">
-        <x:v>140</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="C62" s="0" t="s">
         <x:v>5</x:v>
@@ -1978,10 +1885,10 @@
     </x:row>
     <x:row r="63" spans="1:3">
       <x:c r="A63" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="B63" s="0" t="s">
-        <x:v>142</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="C63" s="0" t="s">
         <x:v>5</x:v>
@@ -1989,10 +1896,10 @@
     </x:row>
     <x:row r="64" spans="1:3">
       <x:c r="A64" s="0" t="s">
-        <x:v>143</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="B64" s="0" t="s">
-        <x:v>144</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="C64" s="0" t="s">
         <x:v>5</x:v>
@@ -2000,10 +1907,10 @@
     </x:row>
     <x:row r="65" spans="1:3">
       <x:c r="A65" s="0" t="s">
-        <x:v>145</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="B65" s="0" t="s">
-        <x:v>146</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="C65" s="0" t="s">
         <x:v>5</x:v>
@@ -2011,10 +1918,10 @@
     </x:row>
     <x:row r="66" spans="1:3">
       <x:c r="A66" s="0" t="s">
-        <x:v>147</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="B66" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="C66" s="0" t="s">
         <x:v>5</x:v>
@@ -2022,10 +1929,10 @@
     </x:row>
     <x:row r="67" spans="1:3">
       <x:c r="A67" s="0" t="s">
-        <x:v>149</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="B67" s="0" t="s">
-        <x:v>150</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="C67" s="0" t="s">
         <x:v>5</x:v>
@@ -2033,10 +1940,10 @@
     </x:row>
     <x:row r="68" spans="1:3">
       <x:c r="A68" s="0" t="s">
-        <x:v>151</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="B68" s="0" t="s">
-        <x:v>152</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="C68" s="0" t="s">
         <x:v>5</x:v>
@@ -2044,10 +1951,10 @@
     </x:row>
     <x:row r="69" spans="1:3">
       <x:c r="A69" s="0" t="s">
-        <x:v>153</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="B69" s="0" t="s">
-        <x:v>154</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="C69" s="0" t="s">
         <x:v>5</x:v>
@@ -2055,10 +1962,10 @@
     </x:row>
     <x:row r="70" spans="1:3">
       <x:c r="A70" s="0" t="s">
-        <x:v>155</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="B70" s="0" t="s">
-        <x:v>156</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="C70" s="0" t="s">
         <x:v>5</x:v>
@@ -2066,10 +1973,10 @@
     </x:row>
     <x:row r="71" spans="1:3">
       <x:c r="A71" s="0" t="s">
-        <x:v>157</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="B71" s="0" t="s">
-        <x:v>158</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="C71" s="0" t="s">
         <x:v>5</x:v>
@@ -2077,10 +1984,10 @@
     </x:row>
     <x:row r="72" spans="1:3">
       <x:c r="A72" s="0" t="s">
-        <x:v>159</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="B72" s="0" t="s">
-        <x:v>160</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="C72" s="0" t="s">
         <x:v>5</x:v>
@@ -2088,167 +1995,167 @@
     </x:row>
     <x:row r="73" spans="1:3">
       <x:c r="A73" s="0" t="s">
-        <x:v>161</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="B73" s="0" t="s">
-        <x:v>162</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="C73" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>149</x:v>
       </x:c>
     </x:row>
     <x:row r="74" spans="1:3">
       <x:c r="A74" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="B74" s="0" t="s">
-        <x:v>164</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="C74" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>152</x:v>
       </x:c>
     </x:row>
     <x:row r="75" spans="1:3">
       <x:c r="A75" s="0" t="s">
-        <x:v>165</x:v>
+        <x:v>153</x:v>
       </x:c>
       <x:c r="B75" s="0" t="s">
-        <x:v>166</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="C75" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>155</x:v>
       </x:c>
     </x:row>
     <x:row r="76" spans="1:3">
       <x:c r="A76" s="0" t="s">
-        <x:v>167</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="B76" s="0" t="s">
-        <x:v>168</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="C76" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>158</x:v>
       </x:c>
     </x:row>
     <x:row r="77" spans="1:3">
       <x:c r="A77" s="0" t="s">
-        <x:v>169</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="B77" s="0" t="s">
-        <x:v>170</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="C77" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>161</x:v>
       </x:c>
     </x:row>
     <x:row r="78" spans="1:3">
       <x:c r="A78" s="0" t="s">
-        <x:v>171</x:v>
+        <x:v>162</x:v>
       </x:c>
       <x:c r="B78" s="0" t="s">
-        <x:v>172</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="C78" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>164</x:v>
       </x:c>
     </x:row>
     <x:row r="79" spans="1:3">
       <x:c r="A79" s="0" t="s">
-        <x:v>173</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="B79" s="0" t="s">
-        <x:v>174</x:v>
+        <x:v>166</x:v>
       </x:c>
       <x:c r="C79" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>167</x:v>
       </x:c>
     </x:row>
     <x:row r="80" spans="1:3">
       <x:c r="A80" s="0" t="s">
-        <x:v>175</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="B80" s="0" t="s">
-        <x:v>176</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="C80" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>170</x:v>
       </x:c>
     </x:row>
     <x:row r="81" spans="1:3">
       <x:c r="A81" s="0" t="s">
-        <x:v>177</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="B81" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>172</x:v>
       </x:c>
       <x:c r="C81" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>173</x:v>
       </x:c>
     </x:row>
     <x:row r="82" spans="1:3">
       <x:c r="A82" s="0" t="s">
-        <x:v>179</x:v>
+        <x:v>174</x:v>
       </x:c>
       <x:c r="B82" s="0" t="s">
-        <x:v>180</x:v>
+        <x:v>175</x:v>
       </x:c>
       <x:c r="C82" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>176</x:v>
       </x:c>
     </x:row>
     <x:row r="83" spans="1:3">
       <x:c r="A83" s="0" t="s">
-        <x:v>181</x:v>
+        <x:v>177</x:v>
       </x:c>
       <x:c r="B83" s="0" t="s">
-        <x:v>182</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="C83" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>179</x:v>
       </x:c>
     </x:row>
     <x:row r="84" spans="1:3">
       <x:c r="A84" s="0" t="s">
-        <x:v>183</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="B84" s="0" t="s">
-        <x:v>184</x:v>
+        <x:v>181</x:v>
       </x:c>
       <x:c r="C84" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>182</x:v>
       </x:c>
     </x:row>
     <x:row r="85" spans="1:3">
       <x:c r="A85" s="0" t="s">
-        <x:v>185</x:v>
+        <x:v>183</x:v>
       </x:c>
       <x:c r="B85" s="0" t="s">
-        <x:v>186</x:v>
+        <x:v>184</x:v>
       </x:c>
       <x:c r="C85" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="86" spans="1:3">
       <x:c r="A86" s="0" t="s">
+        <x:v>185</x:v>
+      </x:c>
+      <x:c r="B86" s="0" t="s">
+        <x:v>186</x:v>
+      </x:c>
+      <x:c r="C86" s="0" t="s">
         <x:v>187</x:v>
-      </x:c>
-      <x:c r="B86" s="0" t="s">
-        <x:v>188</x:v>
-      </x:c>
-      <x:c r="C86" s="0" t="s">
-        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="87" spans="1:3">
       <x:c r="A87" s="0" t="s">
+        <x:v>188</x:v>
+      </x:c>
+      <x:c r="B87" s="0" t="s">
         <x:v>189</x:v>
       </x:c>
-      <x:c r="B87" s="0" t="s">
+      <x:c r="C87" s="0" t="s">
         <x:v>190</x:v>
-      </x:c>
-      <x:c r="C87" s="0" t="s">
-        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="88" spans="1:3">
@@ -2270,7 +2177,7 @@
         <x:v>194</x:v>
       </x:c>
       <x:c r="C89" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="90" spans="1:3">
@@ -2281,15 +2188,15 @@
         <x:v>196</x:v>
       </x:c>
       <x:c r="C90" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>197</x:v>
       </x:c>
     </x:row>
     <x:row r="91" spans="1:3">
       <x:c r="A91" s="0" t="s">
-        <x:v>197</x:v>
+        <x:v>198</x:v>
       </x:c>
       <x:c r="B91" s="0" t="s">
-        <x:v>198</x:v>
+        <x:v>199</x:v>
       </x:c>
       <x:c r="C91" s="0" t="s">
         <x:v>5</x:v>
@@ -2297,21 +2204,21 @@
     </x:row>
     <x:row r="92" spans="1:3">
       <x:c r="A92" s="0" t="s">
-        <x:v>199</x:v>
+        <x:v>200</x:v>
       </x:c>
       <x:c r="B92" s="0" t="s">
-        <x:v>200</x:v>
+        <x:v>201</x:v>
       </x:c>
       <x:c r="C92" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="93" spans="1:3">
       <x:c r="A93" s="0" t="s">
-        <x:v>201</x:v>
+        <x:v>202</x:v>
       </x:c>
       <x:c r="B93" s="0" t="s">
-        <x:v>202</x:v>
+        <x:v>203</x:v>
       </x:c>
       <x:c r="C93" s="0" t="s">
         <x:v>5</x:v>
@@ -2319,10 +2226,10 @@
     </x:row>
     <x:row r="94" spans="1:3">
       <x:c r="A94" s="0" t="s">
-        <x:v>203</x:v>
+        <x:v>204</x:v>
       </x:c>
       <x:c r="B94" s="0" t="s">
-        <x:v>204</x:v>
+        <x:v>205</x:v>
       </x:c>
       <x:c r="C94" s="0" t="s">
         <x:v>5</x:v>
@@ -2330,10 +2237,10 @@
     </x:row>
     <x:row r="95" spans="1:3">
       <x:c r="A95" s="0" t="s">
-        <x:v>205</x:v>
+        <x:v>206</x:v>
       </x:c>
       <x:c r="B95" s="0" t="s">
-        <x:v>206</x:v>
+        <x:v>207</x:v>
       </x:c>
       <x:c r="C95" s="0" t="s">
         <x:v>5</x:v>
@@ -2341,10 +2248,10 @@
     </x:row>
     <x:row r="96" spans="1:3">
       <x:c r="A96" s="0" t="s">
-        <x:v>207</x:v>
+        <x:v>208</x:v>
       </x:c>
       <x:c r="B96" s="0" t="s">
-        <x:v>208</x:v>
+        <x:v>209</x:v>
       </x:c>
       <x:c r="C96" s="0" t="s">
         <x:v>5</x:v>
@@ -2352,10 +2259,10 @@
     </x:row>
     <x:row r="97" spans="1:3">
       <x:c r="A97" s="0" t="s">
-        <x:v>209</x:v>
+        <x:v>210</x:v>
       </x:c>
       <x:c r="B97" s="0" t="s">
-        <x:v>210</x:v>
+        <x:v>211</x:v>
       </x:c>
       <x:c r="C97" s="0" t="s">
         <x:v>5</x:v>
@@ -2363,10 +2270,10 @@
     </x:row>
     <x:row r="98" spans="1:3">
       <x:c r="A98" s="0" t="s">
-        <x:v>211</x:v>
+        <x:v>212</x:v>
       </x:c>
       <x:c r="B98" s="0" t="s">
-        <x:v>212</x:v>
+        <x:v>213</x:v>
       </x:c>
       <x:c r="C98" s="0" t="s">
         <x:v>5</x:v>
@@ -2374,340 +2281,340 @@
     </x:row>
     <x:row r="99" spans="1:3">
       <x:c r="A99" s="0" t="s">
-        <x:v>213</x:v>
+        <x:v>214</x:v>
       </x:c>
       <x:c r="B99" s="0" t="s">
-        <x:v>214</x:v>
+        <x:v>215</x:v>
       </x:c>
       <x:c r="C99" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="100" spans="1:3">
       <x:c r="A100" s="0" t="s">
-        <x:v>215</x:v>
+        <x:v>216</x:v>
       </x:c>
       <x:c r="B100" s="0" t="s">
-        <x:v>216</x:v>
+        <x:v>217</x:v>
       </x:c>
       <x:c r="C100" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="101" spans="1:3">
       <x:c r="A101" s="0" t="s">
-        <x:v>217</x:v>
+        <x:v>218</x:v>
       </x:c>
       <x:c r="B101" s="0" t="s">
-        <x:v>218</x:v>
+        <x:v>219</x:v>
       </x:c>
       <x:c r="C101" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="102" spans="1:3">
       <x:c r="A102" s="0" t="s">
-        <x:v>219</x:v>
+        <x:v>220</x:v>
       </x:c>
       <x:c r="B102" s="0" t="s">
-        <x:v>220</x:v>
+        <x:v>221</x:v>
       </x:c>
       <x:c r="C102" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="103" spans="1:3">
       <x:c r="A103" s="0" t="s">
-        <x:v>221</x:v>
+        <x:v>222</x:v>
       </x:c>
       <x:c r="B103" s="0" t="s">
-        <x:v>222</x:v>
+        <x:v>223</x:v>
       </x:c>
       <x:c r="C103" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="104" spans="1:3">
       <x:c r="A104" s="0" t="s">
-        <x:v>223</x:v>
+        <x:v>224</x:v>
       </x:c>
       <x:c r="B104" s="0" t="s">
-        <x:v>224</x:v>
+        <x:v>225</x:v>
       </x:c>
       <x:c r="C104" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="105" spans="1:3">
       <x:c r="A105" s="0" t="s">
-        <x:v>225</x:v>
+        <x:v>226</x:v>
       </x:c>
       <x:c r="B105" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>227</x:v>
       </x:c>
       <x:c r="C105" s="0" t="s">
-        <x:v>226</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="106" spans="1:3">
       <x:c r="A106" s="0" t="s">
-        <x:v>227</x:v>
+        <x:v>228</x:v>
       </x:c>
       <x:c r="B106" s="0" t="s">
-        <x:v>228</x:v>
+        <x:v>229</x:v>
       </x:c>
       <x:c r="C106" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="107" spans="1:3">
       <x:c r="A107" s="0" t="s">
-        <x:v>229</x:v>
+        <x:v>230</x:v>
       </x:c>
       <x:c r="B107" s="0" t="s">
-        <x:v>230</x:v>
+        <x:v>231</x:v>
       </x:c>
       <x:c r="C107" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="108" spans="1:3">
       <x:c r="A108" s="0" t="s">
-        <x:v>231</x:v>
+        <x:v>232</x:v>
       </x:c>
       <x:c r="B108" s="0" t="s">
-        <x:v>232</x:v>
+        <x:v>233</x:v>
       </x:c>
       <x:c r="C108" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="109" spans="1:3">
       <x:c r="A109" s="0" t="s">
-        <x:v>233</x:v>
+        <x:v>234</x:v>
       </x:c>
       <x:c r="B109" s="0" t="s">
-        <x:v>234</x:v>
+        <x:v>235</x:v>
       </x:c>
       <x:c r="C109" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="110" spans="1:3">
       <x:c r="A110" s="0" t="s">
-        <x:v>235</x:v>
+        <x:v>236</x:v>
       </x:c>
       <x:c r="B110" s="0" t="s">
-        <x:v>236</x:v>
+        <x:v>237</x:v>
       </x:c>
       <x:c r="C110" s="0" t="s">
-        <x:v>237</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="111" spans="1:3">
       <x:c r="A111" s="0" t="s">
+        <x:v>183</x:v>
+      </x:c>
+      <x:c r="B111" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="C111" s="0" t="s">
         <x:v>238</x:v>
-      </x:c>
-      <x:c r="B111" s="0" t="s">
-        <x:v>239</x:v>
-      </x:c>
-      <x:c r="C111" s="0" t="s">
-        <x:v>58</x:v>
       </x:c>
     </x:row>
     <x:row r="112" spans="1:3">
       <x:c r="A112" s="0" t="s">
+        <x:v>239</x:v>
+      </x:c>
+      <x:c r="B112" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="C112" s="0" t="s">
         <x:v>240</x:v>
-      </x:c>
-      <x:c r="B112" s="0" t="s">
-        <x:v>241</x:v>
-      </x:c>
-      <x:c r="C112" s="0" t="s">
-        <x:v>242</x:v>
       </x:c>
     </x:row>
     <x:row r="113" spans="1:3">
       <x:c r="A113" s="0" t="s">
-        <x:v>243</x:v>
+        <x:v>241</x:v>
       </x:c>
       <x:c r="B113" s="0" t="s">
-        <x:v>244</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="C113" s="0" t="s">
-        <x:v>245</x:v>
+        <x:v>242</x:v>
       </x:c>
     </x:row>
     <x:row r="114" spans="1:3">
       <x:c r="A114" s="0" t="s">
-        <x:v>246</x:v>
+        <x:v>243</x:v>
       </x:c>
       <x:c r="B114" s="0" t="s">
-        <x:v>247</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="C114" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>244</x:v>
       </x:c>
     </x:row>
     <x:row r="115" spans="1:3">
       <x:c r="A115" s="0" t="s">
-        <x:v>248</x:v>
+        <x:v>245</x:v>
       </x:c>
       <x:c r="B115" s="0" t="s">
-        <x:v>249</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="C115" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>246</x:v>
       </x:c>
     </x:row>
     <x:row r="116" spans="1:3">
       <x:c r="A116" s="0" t="s">
-        <x:v>250</x:v>
+        <x:v>247</x:v>
       </x:c>
       <x:c r="B116" s="0" t="s">
-        <x:v>251</x:v>
+        <x:v>248</x:v>
       </x:c>
       <x:c r="C116" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="117" spans="1:3">
       <x:c r="A117" s="0" t="s">
-        <x:v>252</x:v>
+        <x:v>249</x:v>
       </x:c>
       <x:c r="B117" s="0" t="s">
-        <x:v>253</x:v>
+        <x:v>250</x:v>
       </x:c>
       <x:c r="C117" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="118" spans="1:3">
       <x:c r="A118" s="0" t="s">
-        <x:v>254</x:v>
+        <x:v>251</x:v>
       </x:c>
       <x:c r="B118" s="0" t="s">
-        <x:v>255</x:v>
+        <x:v>252</x:v>
       </x:c>
       <x:c r="C118" s="0" t="s">
-        <x:v>256</x:v>
+        <x:v>253</x:v>
       </x:c>
     </x:row>
     <x:row r="119" spans="1:3">
       <x:c r="A119" s="0" t="s">
-        <x:v>257</x:v>
+        <x:v>254</x:v>
       </x:c>
       <x:c r="B119" s="0" t="s">
-        <x:v>258</x:v>
+        <x:v>255</x:v>
       </x:c>
       <x:c r="C119" s="0" t="s">
-        <x:v>259</x:v>
+        <x:v>256</x:v>
       </x:c>
     </x:row>
     <x:row r="120" spans="1:3">
       <x:c r="A120" s="0" t="s">
-        <x:v>260</x:v>
+        <x:v>257</x:v>
       </x:c>
       <x:c r="B120" s="0" t="s">
-        <x:v>261</x:v>
+        <x:v>258</x:v>
       </x:c>
       <x:c r="C120" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="121" spans="1:3">
       <x:c r="A121" s="0" t="s">
-        <x:v>262</x:v>
+        <x:v>259</x:v>
       </x:c>
       <x:c r="B121" s="0" t="s">
-        <x:v>263</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="C121" s="0" t="s">
-        <x:v>264</x:v>
+        <x:v>261</x:v>
       </x:c>
     </x:row>
     <x:row r="122" spans="1:3">
       <x:c r="A122" s="0" t="s">
-        <x:v>265</x:v>
+        <x:v>262</x:v>
       </x:c>
       <x:c r="B122" s="0" t="s">
-        <x:v>266</x:v>
+        <x:v>263</x:v>
       </x:c>
       <x:c r="C122" s="0" t="s">
-        <x:v>267</x:v>
+        <x:v>264</x:v>
       </x:c>
     </x:row>
     <x:row r="123" spans="1:3">
       <x:c r="A123" s="0" t="s">
-        <x:v>268</x:v>
+        <x:v>265</x:v>
       </x:c>
       <x:c r="B123" s="0" t="s">
-        <x:v>269</x:v>
+        <x:v>266</x:v>
       </x:c>
       <x:c r="C123" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="124" spans="1:3">
       <x:c r="A124" s="0" t="s">
-        <x:v>270</x:v>
+        <x:v>267</x:v>
       </x:c>
       <x:c r="B124" s="0" t="s">
-        <x:v>271</x:v>
+        <x:v>268</x:v>
       </x:c>
       <x:c r="C124" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="125" spans="1:3">
       <x:c r="A125" s="0" t="s">
-        <x:v>272</x:v>
+        <x:v>269</x:v>
       </x:c>
       <x:c r="B125" s="0" t="s">
-        <x:v>273</x:v>
+        <x:v>270</x:v>
       </x:c>
       <x:c r="C125" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="126" spans="1:3">
       <x:c r="A126" s="0" t="s">
-        <x:v>274</x:v>
+        <x:v>271</x:v>
       </x:c>
       <x:c r="B126" s="0" t="s">
-        <x:v>275</x:v>
+        <x:v>272</x:v>
       </x:c>
       <x:c r="C126" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="127" spans="1:3">
       <x:c r="A127" s="0" t="s">
-        <x:v>276</x:v>
+        <x:v>273</x:v>
       </x:c>
       <x:c r="B127" s="0" t="s">
-        <x:v>277</x:v>
+        <x:v>274</x:v>
       </x:c>
       <x:c r="C127" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="128" spans="1:3">
       <x:c r="A128" s="0" t="s">
-        <x:v>278</x:v>
+        <x:v>275</x:v>
       </x:c>
       <x:c r="B128" s="0" t="s">
-        <x:v>279</x:v>
+        <x:v>276</x:v>
       </x:c>
       <x:c r="C128" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="129" spans="1:3">
       <x:c r="A129" s="0" t="s">
-        <x:v>280</x:v>
+        <x:v>210</x:v>
       </x:c>
       <x:c r="B129" s="0" t="s">
-        <x:v>281</x:v>
+        <x:v>211</x:v>
       </x:c>
       <x:c r="C129" s="0" t="s">
         <x:v>5</x:v>
@@ -2715,10 +2622,10 @@
     </x:row>
     <x:row r="130" spans="1:3">
       <x:c r="A130" s="0" t="s">
-        <x:v>282</x:v>
+        <x:v>212</x:v>
       </x:c>
       <x:c r="B130" s="0" t="s">
-        <x:v>283</x:v>
+        <x:v>213</x:v>
       </x:c>
       <x:c r="C130" s="0" t="s">
         <x:v>5</x:v>
@@ -2726,189 +2633,189 @@
     </x:row>
     <x:row r="131" spans="1:3">
       <x:c r="A131" s="0" t="s">
-        <x:v>284</x:v>
+        <x:v>214</x:v>
       </x:c>
       <x:c r="B131" s="0" t="s">
-        <x:v>285</x:v>
+        <x:v>215</x:v>
       </x:c>
       <x:c r="C131" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="132" spans="1:3">
       <x:c r="A132" s="0" t="s">
-        <x:v>286</x:v>
+        <x:v>216</x:v>
       </x:c>
       <x:c r="B132" s="0" t="s">
-        <x:v>287</x:v>
+        <x:v>217</x:v>
       </x:c>
       <x:c r="C132" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="133" spans="1:3">
       <x:c r="A133" s="0" t="s">
-        <x:v>288</x:v>
+        <x:v>234</x:v>
       </x:c>
       <x:c r="B133" s="0" t="s">
-        <x:v>289</x:v>
+        <x:v>235</x:v>
       </x:c>
       <x:c r="C133" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="134" spans="1:3">
       <x:c r="A134" s="0" t="s">
-        <x:v>290</x:v>
+        <x:v>236</x:v>
       </x:c>
       <x:c r="B134" s="0" t="s">
-        <x:v>291</x:v>
+        <x:v>237</x:v>
       </x:c>
       <x:c r="C134" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="135" spans="1:3">
       <x:c r="A135" s="0" t="s">
-        <x:v>292</x:v>
+        <x:v>222</x:v>
       </x:c>
       <x:c r="B135" s="0" t="s">
-        <x:v>293</x:v>
+        <x:v>223</x:v>
       </x:c>
       <x:c r="C135" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="136" spans="1:3">
       <x:c r="A136" s="0" t="s">
-        <x:v>294</x:v>
+        <x:v>224</x:v>
       </x:c>
       <x:c r="B136" s="0" t="s">
-        <x:v>295</x:v>
+        <x:v>225</x:v>
       </x:c>
       <x:c r="C136" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="137" spans="1:3">
       <x:c r="A137" s="0" t="s">
-        <x:v>296</x:v>
+        <x:v>226</x:v>
       </x:c>
       <x:c r="B137" s="0" t="s">
-        <x:v>297</x:v>
+        <x:v>227</x:v>
       </x:c>
       <x:c r="C137" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="138" spans="1:3">
       <x:c r="A138" s="0" t="s">
-        <x:v>298</x:v>
+        <x:v>230</x:v>
       </x:c>
       <x:c r="B138" s="0" t="s">
-        <x:v>299</x:v>
+        <x:v>231</x:v>
       </x:c>
       <x:c r="C138" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="139" spans="1:3">
       <x:c r="A139" s="0" t="s">
-        <x:v>300</x:v>
+        <x:v>228</x:v>
       </x:c>
       <x:c r="B139" s="0" t="s">
-        <x:v>301</x:v>
+        <x:v>229</x:v>
       </x:c>
       <x:c r="C139" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="140" spans="1:3">
       <x:c r="A140" s="0" t="s">
-        <x:v>302</x:v>
+        <x:v>232</x:v>
       </x:c>
       <x:c r="B140" s="0" t="s">
-        <x:v>303</x:v>
+        <x:v>233</x:v>
       </x:c>
       <x:c r="C140" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="141" spans="1:3">
       <x:c r="A141" s="0" t="s">
-        <x:v>304</x:v>
+        <x:v>220</x:v>
       </x:c>
       <x:c r="B141" s="0" t="s">
-        <x:v>305</x:v>
+        <x:v>221</x:v>
       </x:c>
       <x:c r="C141" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="142" spans="1:3">
       <x:c r="A142" s="0" t="s">
-        <x:v>306</x:v>
+        <x:v>218</x:v>
       </x:c>
       <x:c r="B142" s="0" t="s">
-        <x:v>307</x:v>
+        <x:v>219</x:v>
       </x:c>
       <x:c r="C142" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="143" spans="1:3">
       <x:c r="A143" s="0" t="s">
-        <x:v>300</x:v>
+        <x:v>228</x:v>
       </x:c>
       <x:c r="B143" s="0" t="s">
-        <x:v>301</x:v>
+        <x:v>229</x:v>
       </x:c>
       <x:c r="C143" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="144" spans="1:3">
       <x:c r="A144" s="0" t="s">
-        <x:v>302</x:v>
+        <x:v>232</x:v>
       </x:c>
       <x:c r="B144" s="0" t="s">
-        <x:v>303</x:v>
+        <x:v>233</x:v>
       </x:c>
       <x:c r="C144" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="145" spans="1:3">
       <x:c r="A145" s="0" t="s">
-        <x:v>304</x:v>
+        <x:v>220</x:v>
       </x:c>
       <x:c r="B145" s="0" t="s">
-        <x:v>305</x:v>
+        <x:v>221</x:v>
       </x:c>
       <x:c r="C145" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="146" spans="1:3">
       <x:c r="A146" s="0" t="s">
-        <x:v>306</x:v>
+        <x:v>218</x:v>
       </x:c>
       <x:c r="B146" s="0" t="s">
-        <x:v>307</x:v>
+        <x:v>219</x:v>
       </x:c>
       <x:c r="C146" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="147" spans="1:3">
       <x:c r="A147" s="0" t="s">
-        <x:v>306</x:v>
+        <x:v>218</x:v>
       </x:c>
       <x:c r="B147" s="0" t="s">
-        <x:v>307</x:v>
+        <x:v>219</x:v>
       </x:c>
       <x:c r="C147" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>